<commit_message>
Run some fact calculations again
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A8324F-6CE6-4B6C-A277-350C7CED7C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9132857-48A6-4607-B15A-F08EC7F78E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5720B9E1-D7F9-47BD-8756-C09FD62EA93D}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,10 +696,10 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="9">
-        <v>31.79</v>
+        <v>27.3</v>
       </c>
       <c r="K2" s="9">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>48</v>
@@ -726,32 +726,32 @@
         <v>1730</v>
       </c>
       <c r="E3" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G3" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H3" s="3">
-        <v>1717</v>
+        <v>1726</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="9">
-        <v>0.85</v>
+        <v>8.3699999999999992</v>
       </c>
       <c r="K3" s="9">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="L3" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="11">
-        <v>7.6E-3</v>
+      <c r="M3" s="10">
+        <v>0</v>
       </c>
       <c r="N3" s="9">
-        <v>1717</v>
+        <v>1730</v>
       </c>
       <c r="O3" s="9"/>
     </row>
@@ -769,32 +769,32 @@
         <v>1390</v>
       </c>
       <c r="E4" s="3">
-        <v>3.5</v>
+        <v>4.3</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
         <v>1385</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="9">
-        <v>2.41</v>
+        <v>14.99</v>
       </c>
       <c r="K4" s="9">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M4" s="11">
-        <v>2.06E-2</v>
+      <c r="M4" s="10">
+        <v>0</v>
       </c>
       <c r="N4" s="9">
-        <v>1362</v>
+        <v>1390</v>
       </c>
       <c r="O4" s="9"/>
     </row>
@@ -827,21 +827,23 @@
         <v>1383</v>
       </c>
       <c r="J5" s="9">
-        <v>21.27</v>
+        <v>60.69</v>
       </c>
       <c r="K5" s="9">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="L5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="11">
-        <v>4.4999999999999998E-2</v>
+      <c r="M5" s="10">
+        <v>0</v>
       </c>
       <c r="N5" s="9">
-        <v>1357</v>
-      </c>
-      <c r="O5" s="9"/>
+        <v>1383</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1383</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1673,10 +1675,10 @@
         <v>66848</v>
       </c>
       <c r="J24" s="9">
-        <v>556.23</v>
+        <v>333.02</v>
       </c>
       <c r="K24" s="9">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="L24" s="13" t="s">
         <v>48</v>
@@ -1945,8 +1947,8 @@
       <c r="L30" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="M30" s="11">
-        <v>6.9999999999999999E-4</v>
+      <c r="M30" s="10">
+        <v>0</v>
       </c>
       <c r="N30" s="9">
         <v>1414</v>

</xml_diff>

<commit_message>
Use gap for ESC47
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B27085-3A9F-4F2F-AFE8-386BBEC242EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C6D4D-04ED-4B78-A65E-6DFD1ACA0338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
@@ -608,7 +608,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,20 +996,19 @@
         <v>14832</v>
       </c>
       <c r="E8" s="3">
-        <f>19735+7087+2128+658+200+54+16+4+1</f>
-        <v>29883</v>
+        <v>1.3</v>
       </c>
       <c r="F8" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="4">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="I8" s="3">
-        <v>14641</v>
+        <v>14594</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="8">

</xml_diff>

<commit_message>
Two digits for gap
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D3E5D7-34E3-4515-B9DC-BFF0BA2A7B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F24536D-C350-427F-848F-065350834B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="54">
   <si>
     <t>Sample</t>
   </si>
@@ -193,13 +193,16 @@
   </si>
   <si>
     <t>2316.26</t>
+  </si>
+  <si>
+    <t>LastLB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +213,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -262,8 +273,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -274,7 +286,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -283,7 +294,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,9 +301,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -605,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5720B9E1-D7F9-47BD-8756-C09FD62EA93D}">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,2034 +630,2161 @@
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>17</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>92</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>43</v>
       </c>
       <c r="E2" s="3">
         <v>11.2</v>
       </c>
       <c r="F2" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="G2" s="3">
         <v>17</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="H2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="12">
         <v>0</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>43</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="8">
+      <c r="K2" s="3"/>
+      <c r="L2" s="7">
         <v>27.3</v>
       </c>
-      <c r="L2" s="8">
+      <c r="M2" s="7"/>
+      <c r="N2" s="7">
         <v>36</v>
       </c>
-      <c r="M2" s="8">
+      <c r="O2" s="7">
         <v>17</v>
       </c>
-      <c r="N2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="9">
+      <c r="P2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="8">
         <v>0</v>
       </c>
-      <c r="P2" s="8">
+      <c r="R2" s="7">
         <v>43</v>
       </c>
-      <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="S2" s="7"/>
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>8</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>39</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>1730</v>
       </c>
       <c r="E3" s="3">
         <v>1.3</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
         <v>8</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="H3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="12">
+        <v>2.3174971031286211E-3</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1726</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="7">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7">
+        <v>36</v>
+      </c>
+      <c r="O3" s="7">
+        <v>8</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="8">
         <v>0</v>
       </c>
-      <c r="I3" s="3">
-        <v>1726</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="8">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="L3" s="8">
-        <v>36</v>
-      </c>
-      <c r="M3" s="8">
-        <v>8</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
+      <c r="R3" s="7">
         <v>1730</v>
       </c>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="S3" s="7"/>
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>13</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>65</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1390</v>
       </c>
       <c r="E4" s="3">
         <v>4.3</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>13</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="H4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="12">
+        <v>3.6101083032490976E-3</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1385</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="7">
+        <v>14.99</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7">
+        <v>36</v>
+      </c>
+      <c r="O4" s="7">
+        <v>13</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" s="8">
         <v>0</v>
       </c>
-      <c r="I4" s="3">
-        <v>1385</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="8">
-        <v>14.99</v>
-      </c>
-      <c r="L4" s="8">
-        <v>36</v>
-      </c>
-      <c r="M4" s="8">
-        <v>13</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="9">
-        <v>0</v>
-      </c>
-      <c r="P4" s="8">
+      <c r="R4" s="7">
         <v>1390</v>
       </c>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="S4" s="7"/>
+      <c r="U4" s="11"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>26</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>133</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>1418</v>
       </c>
       <c r="E5" s="3">
         <v>32</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
         <v>26</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="H5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="12">
         <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1383</v>
       </c>
       <c r="J5" s="3">
         <v>1383</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="3">
+        <v>1383</v>
+      </c>
+      <c r="L5" s="7">
         <v>60.69</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="7"/>
+      <c r="N5" s="7">
         <v>36</v>
       </c>
-      <c r="M5" s="8">
+      <c r="O5" s="7">
         <v>26</v>
       </c>
-      <c r="N5" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O5" s="9">
+      <c r="P5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="8">
         <v>0</v>
       </c>
-      <c r="P5" s="8">
+      <c r="R5" s="7">
         <v>1383</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="S5" s="7">
         <v>1383</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="U5" s="11"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
-        <v>48</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="B6" s="5">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5">
         <v>244</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>1399</v>
       </c>
       <c r="E6" s="3">
         <f>51178+14426+3116+440+35+1+1</f>
         <v>69197</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
         <v>7</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.43</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="H6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0.42609582059123341</v>
+      </c>
+      <c r="J6" s="3">
         <v>981</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="8">
+      <c r="K6" s="3"/>
+      <c r="L6" s="7">
         <f>8591+1106+203+33+6+65</f>
         <v>10004</v>
       </c>
-      <c r="L6" s="8">
+      <c r="M6" s="7"/>
+      <c r="N6" s="7">
         <v>36</v>
       </c>
-      <c r="M6" s="8">
+      <c r="O6" s="7">
         <v>7</v>
       </c>
-      <c r="N6" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O6" s="10">
-        <v>0.42609999999999998</v>
-      </c>
-      <c r="P6" s="8">
+      <c r="P6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>0.42609582059123341</v>
+      </c>
+      <c r="R6" s="7">
         <v>981</v>
       </c>
-      <c r="Q6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="S6" s="7"/>
+      <c r="U6" s="11"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>64</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>349</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>62</v>
       </c>
       <c r="E7" s="3">
         <v>1.3</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="H7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="12">
         <v>0</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>62</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="8">
+      <c r="K7" s="3"/>
+      <c r="L7" s="7">
         <v>135.81</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="7"/>
+      <c r="N7" s="7">
         <v>1</v>
       </c>
-      <c r="M7" s="8">
+      <c r="O7" s="7">
         <v>2</v>
       </c>
-      <c r="N7" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O7" s="9">
+      <c r="P7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q7" s="8">
         <v>0</v>
       </c>
-      <c r="P7" s="8">
+      <c r="R7" s="7">
         <v>62</v>
       </c>
-      <c r="Q7" s="8"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="S7" s="7"/>
+      <c r="U7" s="11"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>79</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>414</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>14832</v>
       </c>
       <c r="E8" s="3">
         <v>1.3</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="H8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1.6308071810333013E-2</v>
+      </c>
+      <c r="J8" s="3">
         <v>14594</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="8">
+      <c r="K8" s="3"/>
+      <c r="L8" s="7">
         <v>9.3699999999999992</v>
       </c>
-      <c r="L8" s="8">
+      <c r="M8" s="7"/>
+      <c r="N8" s="7">
         <v>1</v>
       </c>
-      <c r="M8" s="8">
+      <c r="O8" s="7">
         <v>2</v>
       </c>
-      <c r="N8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O8" s="10">
-        <v>1.6299999999999999E-2</v>
-      </c>
-      <c r="P8" s="8">
+      <c r="P8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>1.6308071810333013E-2</v>
+      </c>
+      <c r="R8" s="7">
         <v>14594</v>
       </c>
-      <c r="Q8" s="8"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="S8" s="7"/>
+      <c r="U8" s="11"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>53</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>281</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>6207</v>
       </c>
       <c r="E9" s="3">
         <v>36000</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
         <v>6</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="H9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0.28270303781773093</v>
+      </c>
+      <c r="J9" s="3">
         <v>4839</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="8">
+      <c r="K9" s="3"/>
+      <c r="L9" s="7">
         <f>11248+2596+178+13+69</f>
         <v>14104</v>
       </c>
-      <c r="L9" s="8">
+      <c r="M9" s="7"/>
+      <c r="N9" s="7">
         <v>16</v>
       </c>
-      <c r="M9" s="8">
+      <c r="O9" s="7">
         <v>6</v>
       </c>
-      <c r="N9" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O9" s="10">
-        <v>0.28270000000000001</v>
-      </c>
-      <c r="P9" s="8">
+      <c r="P9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0.28270303781773093</v>
+      </c>
+      <c r="R9" s="7">
         <v>4839</v>
       </c>
-      <c r="Q9" s="8"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="S9" s="7"/>
+      <c r="U9" s="11"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>53</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>274</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>6653</v>
       </c>
       <c r="E10" s="3">
         <v>36000</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
         <v>5</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="I10" s="3">
+      <c r="H10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0.3483988650182408</v>
+      </c>
+      <c r="J10" s="3">
         <v>4934</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="8">
+      <c r="K10" s="3"/>
+      <c r="L10" s="7">
         <f>11740+960+87+7+52</f>
         <v>12846</v>
       </c>
-      <c r="L10" s="8">
+      <c r="M10" s="7"/>
+      <c r="N10" s="7">
         <v>16</v>
       </c>
-      <c r="M10" s="8">
+      <c r="O10" s="7">
         <v>6</v>
       </c>
-      <c r="N10" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O10" s="10">
-        <v>0.3468</v>
-      </c>
-      <c r="P10" s="8">
+      <c r="P10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>0.34676113360323885</v>
+      </c>
+      <c r="R10" s="7">
         <v>4940</v>
       </c>
-      <c r="Q10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="S10" s="7"/>
+      <c r="U10" s="11"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>53</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>281</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>8446</v>
       </c>
       <c r="E11" s="3">
         <v>36000</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3">
         <v>7</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I11" s="3">
+      <c r="H11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="12">
+        <v>0.54547118023787744</v>
+      </c>
+      <c r="J11" s="3">
         <v>5465</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="8">
+      <c r="K11" s="3"/>
+      <c r="L11" s="7">
         <f>4680+743+148+25+6+39</f>
         <v>5641</v>
       </c>
-      <c r="L11" s="8">
+      <c r="M11" s="7"/>
+      <c r="N11" s="7">
         <v>16</v>
       </c>
-      <c r="M11" s="8">
+      <c r="O11" s="7">
         <v>7</v>
       </c>
-      <c r="N11" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O11" s="10">
-        <v>0.54549999999999998</v>
-      </c>
-      <c r="P11" s="8">
+      <c r="P11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0.54547118023787744</v>
+      </c>
+      <c r="R11" s="7">
         <v>5465</v>
       </c>
-      <c r="Q11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="S11" s="7"/>
+      <c r="U11" s="11"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>53</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>275</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>11822</v>
       </c>
       <c r="E12" s="3">
         <v>36000</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
         <v>37</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0.04</v>
-      </c>
-      <c r="I12" s="3">
+      <c r="H12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="12">
+        <v>3.6199491629415374E-2</v>
+      </c>
+      <c r="J12" s="3">
         <v>11409</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="3"/>
+      <c r="L12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="8">
+      <c r="M12" s="7"/>
+      <c r="N12" s="7">
         <v>36</v>
       </c>
-      <c r="M12" s="8">
+      <c r="O12" s="7">
         <v>53</v>
       </c>
-      <c r="N12" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="10">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="P12" s="8">
+      <c r="P12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>2.5382858109823165E-4</v>
+      </c>
+      <c r="R12" s="7">
         <v>11819</v>
       </c>
-      <c r="Q12" s="8"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="S12" s="7"/>
+      <c r="U12" s="11"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>70</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>346</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>32848</v>
       </c>
       <c r="E13" s="3">
         <f>7132+269+5+2</f>
         <v>7408</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
         <v>4</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I13" s="3">
+      <c r="H13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="12">
+        <v>5.4408885179597473E-2</v>
+      </c>
+      <c r="J13" s="3">
         <v>31153</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="8">
+      <c r="K13" s="3"/>
+      <c r="L13" s="7">
         <f>14452+647+31+119</f>
         <v>15249</v>
       </c>
-      <c r="L13" s="8">
+      <c r="M13" s="7"/>
+      <c r="N13" s="7">
         <v>16</v>
       </c>
-      <c r="M13" s="8">
+      <c r="O13" s="7">
         <v>5</v>
       </c>
-      <c r="N13" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O13" s="10">
-        <v>5.3600000000000002E-2</v>
-      </c>
-      <c r="P13" s="8">
+      <c r="P13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>5.3597203066363022E-2</v>
+      </c>
+      <c r="R13" s="7">
         <v>31177</v>
       </c>
-      <c r="Q13" s="8"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="S13" s="7"/>
+      <c r="U13" s="11"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>70</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>351</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>33486</v>
       </c>
       <c r="E14" s="3">
         <f>2555+122+3</f>
         <v>2680</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
         <v>4</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="H14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="12">
+        <v>7.0935141358577453E-2</v>
+      </c>
+      <c r="J14" s="3">
         <v>31268</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="8">
+      <c r="K14" s="3"/>
+      <c r="L14" s="7">
         <f>7279+375+25+114</f>
         <v>7793</v>
       </c>
-      <c r="L14" s="8">
+      <c r="M14" s="7"/>
+      <c r="N14" s="7">
         <v>16</v>
       </c>
-      <c r="M14" s="8">
+      <c r="O14" s="7">
         <v>5</v>
       </c>
-      <c r="N14" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O14" s="10">
-        <v>7.0800000000000002E-2</v>
-      </c>
-      <c r="P14" s="8">
+      <c r="P14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>7.0763917756531194E-2</v>
+      </c>
+      <c r="R14" s="7">
         <v>31273</v>
       </c>
-      <c r="Q14" s="8"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="S14" s="7"/>
+      <c r="U14" s="11"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>70</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>347</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>35309</v>
       </c>
       <c r="E15" s="3">
         <f>42652+6711+789+61</f>
         <v>50213</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
         <v>6</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="H15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="12">
+        <v>9.7234307022995653E-2</v>
+      </c>
+      <c r="J15" s="3">
         <v>32180</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="8">
+      <c r="K15" s="3"/>
+      <c r="L15" s="7">
         <f>6562+754+81+14+56</f>
         <v>7467</v>
       </c>
-      <c r="L15" s="8">
+      <c r="M15" s="7"/>
+      <c r="N15" s="7">
         <v>16</v>
       </c>
-      <c r="M15" s="8">
+      <c r="O15" s="7">
         <v>6</v>
       </c>
-      <c r="N15" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O15" s="10">
-        <v>9.7199999999999995E-2</v>
-      </c>
-      <c r="P15" s="8">
+      <c r="P15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>9.7234307022995653E-2</v>
+      </c>
+      <c r="R15" s="7">
         <v>32180</v>
       </c>
-      <c r="Q15" s="8"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="S15" s="7"/>
+      <c r="U15" s="11"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>70</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>353</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>44497</v>
       </c>
       <c r="E16" s="3">
         <f>18221+15023+11136+7400+4310+2163+900+298+73+11</f>
         <v>59535</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3">
         <v>11</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I16" s="3">
+      <c r="H16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.14127061478878658</v>
+      </c>
+      <c r="J16" s="3">
         <v>38989</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="8">
+      <c r="K16" s="3"/>
+      <c r="L16" s="7">
         <f>4978+4134+2857+2348+1799+1402+1020+916+807+1079+1401+2153+2346+1912+1547+1084+873+710+777+782+1133+1250+1655+1428+1331+826+514+260+117+47+19+8+6+28</f>
         <v>43547</v>
       </c>
-      <c r="L16" s="8">
+      <c r="M16" s="7"/>
+      <c r="N16" s="7">
         <v>36</v>
       </c>
-      <c r="M16" s="8">
+      <c r="O16" s="7">
         <v>22</v>
       </c>
-      <c r="N16" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O16" s="10">
-        <v>6.8599999999999994E-2</v>
-      </c>
-      <c r="P16" s="8">
+      <c r="P16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>6.8611911623439006E-2</v>
+      </c>
+      <c r="R16" s="7">
         <v>41640</v>
       </c>
-      <c r="Q16" s="8"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="S16" s="7"/>
+      <c r="U16" s="11"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>100</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>514</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>33320</v>
       </c>
       <c r="E17" s="3">
         <f>50558+1348+18</f>
         <v>51924</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3">
         <v>4</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0.19</v>
-      </c>
-      <c r="I17" s="3">
+      <c r="H17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0.19242744157749705</v>
+      </c>
+      <c r="J17" s="3">
         <v>27943</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="8">
+      <c r="K17" s="3"/>
+      <c r="L17" s="7">
         <f>4405+119+350</f>
         <v>4874</v>
       </c>
-      <c r="L17" s="8">
+      <c r="M17" s="7"/>
+      <c r="N17" s="7">
         <v>16</v>
       </c>
-      <c r="M17" s="8">
+      <c r="O17" s="7">
         <v>4</v>
       </c>
-      <c r="N17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O17" s="10">
-        <v>0.19239999999999999</v>
-      </c>
-      <c r="P17" s="8">
+      <c r="P17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0.19242744157749705</v>
+      </c>
+      <c r="R17" s="7">
         <v>27943</v>
       </c>
-      <c r="Q17" s="8"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="S17" s="7"/>
+      <c r="U17" s="11"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>100</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>524</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>35321</v>
       </c>
       <c r="E18" s="3">
         <f>24942+815+13</f>
         <v>25770</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3">
         <v>4</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="I18" s="3">
+      <c r="H18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0.25451962351269758</v>
+      </c>
+      <c r="J18" s="3">
         <v>28155</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="8">
+      <c r="K18" s="3"/>
+      <c r="L18" s="7">
         <f>2173+86+301</f>
         <v>2560</v>
       </c>
-      <c r="L18" s="8">
+      <c r="M18" s="7"/>
+      <c r="N18" s="7">
         <v>16</v>
       </c>
-      <c r="M18" s="8">
+      <c r="O18" s="7">
         <v>4</v>
       </c>
-      <c r="N18" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O18" s="10">
-        <v>0.2545</v>
-      </c>
-      <c r="P18" s="8">
+      <c r="P18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>0.25451962351269758</v>
+      </c>
+      <c r="R18" s="7">
         <v>28155</v>
       </c>
-      <c r="Q18" s="8"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="S18" s="7"/>
+      <c r="U18" s="11"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>100</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>534</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>41340</v>
       </c>
       <c r="E19" s="3">
         <f>28940+2746+170+6</f>
         <v>31862</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3">
         <v>5</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0.46</v>
-      </c>
-      <c r="I19" s="3">
+      <c r="H19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="12">
+        <v>0.4553263395057382</v>
+      </c>
+      <c r="J19" s="3">
         <v>28406</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="8">
+      <c r="K19" s="3"/>
+      <c r="L19" s="7">
         <f>2723+258+31+124</f>
         <v>3136</v>
       </c>
-      <c r="L19" s="8">
+      <c r="M19" s="7"/>
+      <c r="N19" s="7">
         <v>16</v>
       </c>
-      <c r="M19" s="8">
+      <c r="O19" s="7">
         <v>5</v>
       </c>
-      <c r="N19" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O19" s="10">
-        <v>0.45529999999999998</v>
-      </c>
-      <c r="P19" s="8">
+      <c r="P19" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>0.4553263395057382</v>
+      </c>
+      <c r="R19" s="7">
         <v>28406</v>
       </c>
-      <c r="Q19" s="8"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="S19" s="7"/>
+      <c r="U19" s="11"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>100</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>526</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>62818</v>
       </c>
       <c r="E20" s="3">
         <f>32570+8971+2042+349+40+3</f>
         <v>43975</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
         <v>7</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0.64</v>
-      </c>
-      <c r="I20" s="3">
+      <c r="H20" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0.63724979149291072</v>
+      </c>
+      <c r="J20" s="3">
         <v>38368</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="8">
+      <c r="K20" s="3"/>
+      <c r="L20" s="7">
         <f>19275+3421+743+168+3512+55</f>
         <v>27174</v>
       </c>
-      <c r="L20" s="8">
+      <c r="M20" s="7"/>
+      <c r="N20" s="7">
         <v>16</v>
       </c>
-      <c r="M20" s="8">
+      <c r="O20" s="7">
         <v>8</v>
       </c>
-      <c r="N20" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O20" s="10">
-        <v>0.63119999999999998</v>
-      </c>
-      <c r="P20" s="8">
+      <c r="P20" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>0.63117031497494225</v>
+      </c>
+      <c r="R20" s="7">
         <v>38511</v>
       </c>
-      <c r="Q20" s="8"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="S20" s="7"/>
+      <c r="U20" s="11"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>43</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>203</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>22545</v>
       </c>
       <c r="E21" s="3">
         <f>5164+498+33+1</f>
         <v>5696</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
         <v>5</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="4">
-        <v>29.55</v>
-      </c>
-      <c r="I21" s="3">
+      <c r="H21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="12">
+        <v>29.548780487804876</v>
+      </c>
+      <c r="J21" s="3">
         <v>738</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="8">
+      <c r="K21" s="3"/>
+      <c r="L21" s="7">
         <f>6083+412+40+5+55</f>
         <v>6595</v>
       </c>
-      <c r="L21" s="8">
+      <c r="M21" s="7"/>
+      <c r="N21" s="7">
         <v>36</v>
       </c>
-      <c r="M21" s="8">
+      <c r="O21" s="7">
         <v>6</v>
       </c>
-      <c r="N21" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O21" s="9">
-        <v>27.61</v>
-      </c>
-      <c r="P21" s="8">
+      <c r="P21" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>27.610406091370557</v>
+      </c>
+      <c r="R21" s="7">
         <v>788</v>
       </c>
-      <c r="Q21" s="8"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="S21" s="7"/>
+      <c r="U21" s="11"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>43</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>198</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>22841</v>
       </c>
       <c r="E22" s="3">
         <f>8482+1495+192+17</f>
         <v>10186</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3">
         <v>6</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="4">
-        <v>29.52</v>
-      </c>
-      <c r="I22" s="3">
+      <c r="H22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="12">
+        <v>29.495327102803738</v>
+      </c>
+      <c r="J22" s="3">
         <v>749</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="8">
+      <c r="K22" s="3"/>
+      <c r="L22" s="7">
         <f>11046+798+106+16+4+38</f>
         <v>12008</v>
       </c>
-      <c r="L22" s="8">
+      <c r="M22" s="7"/>
+      <c r="N22" s="7">
         <v>36</v>
       </c>
-      <c r="M22" s="8">
+      <c r="O22" s="7">
         <v>7</v>
       </c>
-      <c r="N22" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O22" s="9">
-        <v>25.04</v>
-      </c>
-      <c r="P22" s="8">
+      <c r="P22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>25.044469783352337</v>
+      </c>
+      <c r="R22" s="7">
         <v>877</v>
       </c>
-      <c r="Q22" s="8"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="S22" s="7"/>
+      <c r="U22" s="11"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>43</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>211</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>23122</v>
       </c>
       <c r="E23" s="3">
         <f>7476+2800+887+239+48+7</f>
         <v>11457</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="3"/>
+      <c r="G23" s="3">
         <v>9</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="4">
-        <v>26.23</v>
-      </c>
-      <c r="I23" s="3">
+      <c r="H23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="12">
+        <v>24.748329621380847</v>
+      </c>
+      <c r="J23" s="3">
         <v>898</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="8">
+      <c r="K23" s="3"/>
+      <c r="L23" s="7">
         <f>4910+1142+256+71+21+7+3+25</f>
         <v>6435</v>
       </c>
-      <c r="L23" s="8">
+      <c r="M23" s="7"/>
+      <c r="N23" s="7">
         <v>36</v>
       </c>
-      <c r="M23" s="8">
+      <c r="O23" s="7">
         <v>9</v>
       </c>
-      <c r="N23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O23" s="9">
-        <v>24.52</v>
-      </c>
-      <c r="P23" s="8">
+      <c r="P23" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>24.520971302428258</v>
+      </c>
+      <c r="R23" s="7">
         <v>906</v>
       </c>
-      <c r="Q23" s="8"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="S23" s="7"/>
+      <c r="U23" s="11"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>43</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>204</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>66857</v>
       </c>
       <c r="E24" s="3">
         <v>4470</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3">
         <v>43</v>
       </c>
-      <c r="G24" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H24" s="4">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
+      <c r="H24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="12">
+        <v>2.9919516500613349E-5</v>
+      </c>
+      <c r="J24" s="3">
         <v>66846</v>
       </c>
-      <c r="J24" s="3">
+      <c r="K24" s="3">
         <v>66848</v>
       </c>
-      <c r="K24" s="8">
+      <c r="L24" s="7">
         <v>333.02</v>
       </c>
-      <c r="L24" s="8">
+      <c r="M24" s="7"/>
+      <c r="N24" s="7">
         <v>36</v>
       </c>
-      <c r="M24" s="8">
+      <c r="O24" s="7">
         <v>43</v>
       </c>
-      <c r="N24" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O24" s="10">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="P24" s="8">
+      <c r="P24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>2.9919516500613349E-5</v>
+      </c>
+      <c r="R24" s="7">
         <v>66846</v>
       </c>
-      <c r="Q24" s="8">
+      <c r="S24" s="7">
         <v>66848</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="U24" s="11"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>99</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>510</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>1474</v>
       </c>
       <c r="E25" s="3">
         <f>18100+645+12</f>
         <v>18757</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3">
         <v>4</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="4">
-        <v>1.33</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="H25" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25" s="12">
+        <v>1.3322784810126582</v>
+      </c>
+      <c r="J25" s="3">
         <v>632</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="8">
+      <c r="K25" s="3"/>
+      <c r="L25" s="7">
         <f>1782+72+260</f>
         <v>2114</v>
       </c>
-      <c r="L25" s="8">
+      <c r="M25" s="7"/>
+      <c r="N25" s="7">
         <v>16</v>
       </c>
-      <c r="M25" s="8">
+      <c r="O25" s="7">
         <v>4</v>
       </c>
-      <c r="N25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O25" s="10">
-        <v>1.3323</v>
-      </c>
-      <c r="P25" s="8">
+      <c r="P25" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>1.3322784810126582</v>
+      </c>
+      <c r="R25" s="7">
         <v>632</v>
       </c>
-      <c r="Q25" s="8"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="S25" s="7"/>
+      <c r="U25" s="11"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>41</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>208</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>232</v>
       </c>
       <c r="E26" s="3">
         <f>7107+1428+224+24+1</f>
         <v>8784</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
         <v>7</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="4">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I26" s="3">
+      <c r="H26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I26" s="12">
+        <v>0.55704697986577179</v>
+      </c>
+      <c r="J26" s="3">
         <v>149</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="8">
+      <c r="K26" s="3"/>
+      <c r="L26" s="7">
         <f>47056+4159+438+77+13+4+47</f>
         <v>51794</v>
       </c>
-      <c r="L26" s="8">
+      <c r="M26" s="7"/>
+      <c r="N26" s="7">
         <v>36</v>
       </c>
-      <c r="M26" s="8">
+      <c r="O26" s="7">
         <v>7</v>
       </c>
-      <c r="N26" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O26" s="10">
-        <v>0.51629999999999998</v>
-      </c>
-      <c r="P26" s="8">
+      <c r="P26" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>0.5163398692810458</v>
+      </c>
+      <c r="R26" s="7">
         <v>153</v>
       </c>
-      <c r="Q26" s="8"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="S26" s="7"/>
+      <c r="U26" s="11"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="6">
-        <v>49</v>
-      </c>
-      <c r="C27" s="6">
+      <c r="B27" s="5">
+        <v>49</v>
+      </c>
+      <c r="C27" s="5">
         <v>255</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>282</v>
       </c>
       <c r="E27" s="3">
         <v>0.9</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
         <v>1</v>
       </c>
-      <c r="G27" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" s="4">
-        <v>0.04</v>
-      </c>
-      <c r="I27" s="3">
+      <c r="H27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="12">
+        <v>3.6764705882352942E-2</v>
+      </c>
+      <c r="J27" s="3">
         <v>272</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="8">
+      <c r="K27" s="3"/>
+      <c r="L27" s="7">
         <v>8.34</v>
       </c>
-      <c r="L27" s="8">
+      <c r="M27" s="7"/>
+      <c r="N27" s="7">
         <v>1</v>
       </c>
-      <c r="M27" s="8">
+      <c r="O27" s="7">
         <v>2</v>
       </c>
-      <c r="N27" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O27" s="10">
-        <v>3.6799999999999999E-2</v>
-      </c>
-      <c r="P27" s="8">
+      <c r="P27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>3.6764705882352942E-2</v>
+      </c>
+      <c r="R27" s="7">
         <v>272</v>
       </c>
-      <c r="Q27" s="8"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="S27" s="7"/>
+      <c r="U27" s="11"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>51</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>259</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>378</v>
       </c>
       <c r="E28" s="3">
         <v>0.2</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3">
         <v>1</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="I28" s="3">
+      <c r="H28" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="12">
+        <v>1.6129032258064516E-2</v>
+      </c>
+      <c r="J28" s="3">
         <v>372</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="8">
+      <c r="K28" s="3"/>
+      <c r="L28" s="7">
         <v>7.02</v>
       </c>
-      <c r="L28" s="8">
+      <c r="M28" s="7"/>
+      <c r="N28" s="7">
         <v>1</v>
       </c>
-      <c r="M28" s="8">
+      <c r="O28" s="7">
         <v>2</v>
       </c>
-      <c r="N28" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O28" s="10">
-        <v>1.61E-2</v>
-      </c>
-      <c r="P28" s="8">
+      <c r="P28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>1.6129032258064516E-2</v>
+      </c>
+      <c r="R28" s="7">
         <v>372</v>
       </c>
-      <c r="Q28" s="8"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="S28" s="7"/>
+      <c r="U28" s="11"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>110</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>573</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>848</v>
       </c>
       <c r="E29" s="3">
         <v>2407</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3">
         <v>50</v>
       </c>
-      <c r="G29" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H29" s="4">
-        <v>0.04</v>
-      </c>
-      <c r="I29" s="3">
+      <c r="H29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="12">
+        <v>4.4334975369458129E-2</v>
+      </c>
+      <c r="J29" s="3">
         <v>812</v>
       </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="8">
+      <c r="K29" s="3"/>
+      <c r="L29" s="7">
         <v>1225.27</v>
       </c>
-      <c r="L29" s="8">
+      <c r="M29" s="7"/>
+      <c r="N29" s="7">
         <v>16</v>
       </c>
-      <c r="M29" s="8">
+      <c r="O29" s="7">
         <v>110</v>
       </c>
-      <c r="N29" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O29" s="9">
+      <c r="P29" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q29" s="8">
         <v>0</v>
       </c>
-      <c r="P29" s="8">
+      <c r="R29" s="7">
         <v>848</v>
       </c>
-      <c r="Q29" s="8"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="S29" s="7"/>
+      <c r="U29" s="11"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>151</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>871</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>1415</v>
       </c>
       <c r="E30" s="3">
         <v>0.4</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
         <v>1</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H30" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I30" s="3">
+      <c r="H30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" s="12">
+        <v>4.5824094604582408E-2</v>
+      </c>
+      <c r="J30" s="3">
         <v>1353</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="8">
+      <c r="K30" s="3"/>
+      <c r="L30" s="7">
         <v>3005.15</v>
       </c>
-      <c r="L30" s="8">
+      <c r="M30" s="7"/>
+      <c r="N30" s="7">
         <v>16</v>
       </c>
-      <c r="M30" s="8">
+      <c r="O30" s="7">
         <v>151</v>
       </c>
-      <c r="N30" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O30" s="9">
+      <c r="P30" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q30" s="8">
         <v>0</v>
       </c>
-      <c r="P30" s="8">
+      <c r="R30" s="7">
         <v>1414</v>
       </c>
-      <c r="Q30" s="8">
+      <c r="S30" s="7">
         <v>1414</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="U30" s="11"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>175</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>962</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>1644</v>
       </c>
       <c r="E31" s="3">
         <v>0.4</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="3"/>
+      <c r="G31" s="3">
         <v>1</v>
       </c>
-      <c r="G31" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H31" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I31" s="3">
+      <c r="H31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="12">
+        <v>4.8469387755102039E-2</v>
+      </c>
+      <c r="J31" s="3">
         <v>1568</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="8">
+      <c r="K31" s="3"/>
+      <c r="L31" s="7">
         <v>65.099999999999994</v>
       </c>
-      <c r="L31" s="8">
+      <c r="M31" s="7"/>
+      <c r="N31" s="7">
         <v>1</v>
       </c>
-      <c r="M31" s="8">
+      <c r="O31" s="7">
         <v>2</v>
       </c>
-      <c r="N31" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O31" s="10">
-        <v>4.8500000000000001E-2</v>
-      </c>
-      <c r="P31" s="8">
+      <c r="P31" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>4.8469387755102039E-2</v>
+      </c>
+      <c r="R31" s="7">
         <v>1568</v>
       </c>
-      <c r="Q31" s="8"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="S31" s="7"/>
+      <c r="U31" s="11"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>254</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>1389</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>2376</v>
       </c>
       <c r="E32" s="3">
         <v>0.8</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="3"/>
+      <c r="G32" s="3">
         <v>1</v>
       </c>
-      <c r="G32" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H32" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="I32" s="3">
+      <c r="H32" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I32" s="12">
+        <v>4.7157338034376377E-2</v>
+      </c>
+      <c r="J32" s="3">
         <v>2269</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="8">
+      <c r="K32" s="3"/>
+      <c r="L32" s="7">
         <v>186.81</v>
       </c>
-      <c r="L32" s="8">
+      <c r="M32" s="7"/>
+      <c r="N32" s="7">
         <v>1</v>
       </c>
-      <c r="M32" s="8">
+      <c r="O32" s="7">
         <v>2</v>
       </c>
-      <c r="N32" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O32" s="10">
-        <v>4.7199999999999999E-2</v>
-      </c>
-      <c r="P32" s="8">
+      <c r="P32" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>4.7157338034376377E-2</v>
+      </c>
+      <c r="R32" s="7">
         <v>2269</v>
       </c>
-      <c r="Q32" s="8"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="S32" s="7"/>
+      <c r="U32" s="11"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>324</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>1825</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>2547</v>
       </c>
       <c r="E33" s="3">
         <v>2</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3">
         <v>1</v>
       </c>
-      <c r="G33" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H33" s="4">
-        <v>0.04</v>
-      </c>
-      <c r="I33" s="3">
+      <c r="H33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="12">
+        <v>4.0441176470588237E-2</v>
+      </c>
+      <c r="J33" s="3">
         <v>2448</v>
       </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="8">
+      <c r="K33" s="3"/>
+      <c r="L33" s="7">
         <v>431.65</v>
       </c>
-      <c r="L33" s="8">
+      <c r="M33" s="7"/>
+      <c r="N33" s="7">
         <v>1</v>
       </c>
-      <c r="M33" s="8">
+      <c r="O33" s="7">
         <v>2</v>
       </c>
-      <c r="N33" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O33" s="10">
-        <v>4.0399999999999998E-2</v>
-      </c>
-      <c r="P33" s="8">
+      <c r="P33" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>4.0441176470588237E-2</v>
+      </c>
+      <c r="R33" s="7">
         <v>2448</v>
       </c>
-      <c r="Q33" s="8"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="S33" s="7"/>
+      <c r="U33" s="11"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>342</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>1822</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>2101</v>
       </c>
       <c r="E34" s="3">
         <f>39404+12782+3093+464+44+7</f>
         <v>55794</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="3"/>
+      <c r="G34" s="3">
         <v>7</v>
       </c>
-      <c r="G34" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H34" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I34" s="3">
+      <c r="H34" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I34" s="12">
+        <v>0.14184782608695654</v>
+      </c>
+      <c r="J34" s="3">
         <v>1840</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="8">
+      <c r="K34" s="3"/>
+      <c r="L34" s="7">
         <f>225+198+288</f>
         <v>711</v>
       </c>
-      <c r="L34" s="8">
+      <c r="M34" s="7"/>
+      <c r="N34" s="7">
         <v>16</v>
       </c>
-      <c r="M34" s="8">
+      <c r="O34" s="7">
         <v>4</v>
       </c>
-      <c r="N34" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O34" s="10">
-        <v>0.14180000000000001</v>
-      </c>
-      <c r="P34" s="8">
+      <c r="P34" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>0.14184782608695654</v>
+      </c>
+      <c r="R34" s="7">
         <v>1840</v>
       </c>
-      <c r="Q34" s="8"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="S34" s="7"/>
+      <c r="U34" s="11"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>359</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="5">
         <v>1967</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>2080</v>
       </c>
       <c r="E35" s="3">
         <f>38573+12766+3355+563+40+7+15+7+3</f>
         <v>55329</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="3"/>
+      <c r="G35" s="3">
         <v>9</v>
       </c>
-      <c r="G35" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H35" s="4">
-        <v>0.08</v>
-      </c>
-      <c r="I35" s="3">
+      <c r="H35" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" s="12">
+        <v>7.6047594412829794E-2</v>
+      </c>
+      <c r="J35" s="3">
         <v>1933</v>
       </c>
-      <c r="J35" s="3"/>
-      <c r="K35" s="8">
+      <c r="K35" s="3"/>
+      <c r="L35" s="7">
         <f>328+321+333+438</f>
         <v>1420</v>
       </c>
-      <c r="L35" s="8">
+      <c r="M35" s="7"/>
+      <c r="N35" s="7">
         <v>12</v>
       </c>
-      <c r="M35" s="8">
+      <c r="O35" s="7">
         <v>5</v>
       </c>
-      <c r="N35" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O35" s="10">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="P35" s="8">
+      <c r="P35" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>7.6047594412829794E-2</v>
+      </c>
+      <c r="R35" s="7">
         <v>1933</v>
       </c>
-      <c r="Q35" s="8"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="S35" s="7"/>
+      <c r="U35" s="11"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>379</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="5">
         <v>1973</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>2307</v>
       </c>
       <c r="E36" s="3">
         <f>18532+4458+724+50+11+17+8+3</f>
         <v>23803</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="3"/>
+      <c r="G36" s="3">
         <v>8</v>
       </c>
-      <c r="G36" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H36" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I36" s="3">
+      <c r="H36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I36" s="12">
+        <v>0.13533464566929135</v>
+      </c>
+      <c r="J36" s="3">
         <v>2032</v>
       </c>
-      <c r="J36" s="3"/>
-      <c r="K36" s="8">
+      <c r="K36" s="3"/>
+      <c r="L36" s="7">
         <f>262+268+267+346</f>
         <v>1143</v>
       </c>
-      <c r="L36" s="8">
+      <c r="M36" s="7"/>
+      <c r="N36" s="7">
         <v>11</v>
       </c>
-      <c r="M36" s="8">
+      <c r="O36" s="7">
         <v>4</v>
       </c>
-      <c r="N36" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O36" s="10">
-        <v>0.13589999999999999</v>
-      </c>
-      <c r="P36" s="8">
+      <c r="P36" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q36" s="8">
+        <v>0.13589364844903989</v>
+      </c>
+      <c r="R36" s="7">
         <v>2031</v>
       </c>
-      <c r="Q36" s="8"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="S36" s="7"/>
+      <c r="U36" s="11"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="6">
-        <v>48</v>
-      </c>
-      <c r="C37" s="6">
+      <c r="B37" s="5">
+        <v>48</v>
+      </c>
+      <c r="C37" s="5">
         <v>256</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>13135</v>
       </c>
       <c r="E37" s="3">
         <f>9463+869+51+2</f>
         <v>10385</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="3"/>
+      <c r="G37" s="3">
         <v>5</v>
       </c>
-      <c r="G37" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="I37" s="3">
+      <c r="H37" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I37" s="12">
+        <v>0.22311202160350127</v>
+      </c>
+      <c r="J37" s="3">
         <v>10739</v>
       </c>
-      <c r="J37" s="3"/>
-      <c r="K37" s="8">
+      <c r="K37" s="3"/>
+      <c r="L37" s="7">
         <f>28032+1690+128+12+65</f>
         <v>29927</v>
       </c>
-      <c r="L37" s="8">
+      <c r="M37" s="7"/>
+      <c r="N37" s="7">
         <v>16</v>
       </c>
-      <c r="M37" s="8">
+      <c r="O37" s="7">
         <v>6</v>
       </c>
-      <c r="N37" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O37" s="10">
-        <v>0.2203</v>
-      </c>
-      <c r="P37" s="8">
+      <c r="P37" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q37" s="8">
+        <v>0.2202712746191007</v>
+      </c>
+      <c r="R37" s="7">
         <v>10764</v>
       </c>
-      <c r="Q37" s="8"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="S37" s="7"/>
+      <c r="U37" s="11"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="6">
-        <v>48</v>
-      </c>
-      <c r="C38" s="6">
+      <c r="B38" s="5">
+        <v>48</v>
+      </c>
+      <c r="C38" s="5">
         <v>250</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>13802</v>
       </c>
       <c r="E38" s="3">
         <f>15553+2465+281+20+2</f>
         <v>18321</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="3"/>
+      <c r="G38" s="3">
         <v>6</v>
       </c>
-      <c r="G38" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H38" s="4">
-        <v>0.26</v>
-      </c>
-      <c r="I38" s="3">
+      <c r="H38" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I38" s="12">
+        <v>0.26484604105571846</v>
+      </c>
+      <c r="J38" s="3">
         <v>10912</v>
       </c>
-      <c r="J38" s="3"/>
-      <c r="K38" s="8">
+      <c r="K38" s="3"/>
+      <c r="L38" s="7">
         <f>3939+412+45+6+42</f>
         <v>4444</v>
       </c>
-      <c r="L38" s="8">
+      <c r="M38" s="7"/>
+      <c r="N38" s="7">
         <v>16</v>
       </c>
-      <c r="M38" s="8">
+      <c r="O38" s="7">
         <v>6</v>
       </c>
-      <c r="N38" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O38" s="10">
-        <v>0.25469999999999998</v>
-      </c>
-      <c r="P38" s="8">
+      <c r="P38" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>0.25472727272727275</v>
+      </c>
+      <c r="R38" s="7">
         <v>11000</v>
       </c>
-      <c r="Q38" s="8"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="S38" s="7"/>
+      <c r="U38" s="11"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="6">
-        <v>48</v>
-      </c>
-      <c r="C39" s="6">
+      <c r="B39" s="5">
+        <v>48</v>
+      </c>
+      <c r="C39" s="5">
         <v>254</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>16540</v>
       </c>
       <c r="E39" s="3">
         <f>6822+1934+449+77+9+2</f>
         <v>9293</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="3"/>
+      <c r="G39" s="3">
         <v>7</v>
       </c>
-      <c r="G39" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H39" s="4">
-        <v>0.41</v>
-      </c>
-      <c r="I39" s="3">
+      <c r="H39" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I39" s="12">
+        <v>0.40981929764745995</v>
+      </c>
+      <c r="J39" s="3">
         <v>11732</v>
       </c>
-      <c r="J39" s="3"/>
-      <c r="K39" s="8">
+      <c r="K39" s="3"/>
+      <c r="L39" s="7">
         <f>7879+1078+180+38+9+5+34</f>
         <v>9223</v>
       </c>
-      <c r="L39" s="8">
+      <c r="M39" s="7"/>
+      <c r="N39" s="7">
         <v>36</v>
       </c>
-      <c r="M39" s="8">
+      <c r="O39" s="7">
         <v>8</v>
       </c>
-      <c r="N39" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O39" s="10">
-        <v>0.39910000000000001</v>
-      </c>
-      <c r="P39" s="8">
+      <c r="P39" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>0.39908644899340212</v>
+      </c>
+      <c r="R39" s="7">
         <v>11822</v>
       </c>
-      <c r="Q39" s="8"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="S39" s="7"/>
+      <c r="U39" s="11"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="6">
-        <v>48</v>
-      </c>
-      <c r="C40" s="6">
+      <c r="B40" s="5">
+        <v>48</v>
+      </c>
+      <c r="C40" s="5">
         <v>249</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>25977</v>
       </c>
       <c r="E40" s="3">
         <v>18677</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="3"/>
+      <c r="G40" s="3">
         <v>40</v>
       </c>
-      <c r="G40" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H40" s="4">
-        <v>0.04</v>
-      </c>
-      <c r="I40" s="3">
+      <c r="H40" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I40" s="12">
+        <v>3.7544434237328755E-2</v>
+      </c>
+      <c r="J40" s="3">
         <v>25037</v>
       </c>
-      <c r="J40" s="3"/>
-      <c r="K40" s="8">
+      <c r="K40" s="3"/>
+      <c r="L40" s="7">
         <v>1433.11</v>
       </c>
-      <c r="L40" s="8">
+      <c r="M40" s="7"/>
+      <c r="N40" s="7">
         <v>16</v>
       </c>
-      <c r="M40" s="8">
-        <v>48</v>
-      </c>
-      <c r="N40" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O40" s="9">
+      <c r="O40" s="7">
+        <v>48</v>
+      </c>
+      <c r="P40" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q40" s="8">
         <v>0</v>
       </c>
-      <c r="P40" s="8">
+      <c r="R40" s="7">
         <v>25977</v>
       </c>
-      <c r="Q40" s="8"/>
+      <c r="S40" s="7"/>
+      <c r="U40" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Start fill LB update time
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F24536D-C350-427F-848F-065350834B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F1D277-7D82-4740-8593-8A6A95F57F62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="53">
   <si>
     <t>Sample</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>Layers</t>
-  </si>
-  <si>
-    <t>2316.26</t>
   </si>
   <si>
     <t>LastLB</t>
@@ -620,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5720B9E1-D7F9-47BD-8756-C09FD62EA93D}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +658,7 @@
         <v>43</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>51</v>
@@ -682,7 +679,7 @@
         <v>43</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>50</v>
@@ -738,7 +735,9 @@
       <c r="L2" s="7">
         <v>27.3</v>
       </c>
-      <c r="M2" s="7"/>
+      <c r="M2" s="7">
+        <v>27.3</v>
+      </c>
       <c r="N2" s="7">
         <v>36</v>
       </c>
@@ -773,7 +772,9 @@
       <c r="E3" s="3">
         <v>1.3</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <v>1.3</v>
+      </c>
       <c r="G3" s="3">
         <v>8</v>
       </c>
@@ -790,7 +791,9 @@
       <c r="L3" s="7">
         <v>8.3699999999999992</v>
       </c>
-      <c r="M3" s="7"/>
+      <c r="M3" s="7">
+        <v>8.3699999999999992</v>
+      </c>
       <c r="N3" s="7">
         <v>36</v>
       </c>
@@ -825,7 +828,9 @@
       <c r="E4" s="3">
         <v>4.3</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3">
+        <v>4.3</v>
+      </c>
       <c r="G4" s="3">
         <v>13</v>
       </c>
@@ -842,7 +847,9 @@
       <c r="L4" s="7">
         <v>14.99</v>
       </c>
-      <c r="M4" s="7"/>
+      <c r="M4" s="7">
+        <v>14.99</v>
+      </c>
       <c r="N4" s="7">
         <v>36</v>
       </c>
@@ -877,7 +884,9 @@
       <c r="E5" s="3">
         <v>32</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <v>32</v>
+      </c>
       <c r="G5" s="3">
         <v>26</v>
       </c>
@@ -896,7 +905,9 @@
       <c r="L5" s="7">
         <v>60.69</v>
       </c>
-      <c r="M5" s="7"/>
+      <c r="M5" s="7">
+        <v>60.69</v>
+      </c>
       <c r="N5" s="7">
         <v>36</v>
       </c>
@@ -931,10 +942,12 @@
         <v>1399</v>
       </c>
       <c r="E6" s="3">
+        <v>72000</v>
+      </c>
+      <c r="F6" s="3">
         <f>51178+14426+3116+440+35+1+1</f>
         <v>69197</v>
       </c>
-      <c r="F6" s="3"/>
       <c r="G6" s="3">
         <v>7</v>
       </c>
@@ -952,7 +965,10 @@
         <f>8591+1106+203+33+6+65</f>
         <v>10004</v>
       </c>
-      <c r="M6" s="7"/>
+      <c r="M6" s="7">
+        <f>8591+1106+203+33+6+65</f>
+        <v>10004</v>
+      </c>
       <c r="N6" s="7">
         <v>36</v>
       </c>
@@ -987,7 +1003,9 @@
       <c r="E7" s="3">
         <v>1.3</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>1.3</v>
+      </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
@@ -1004,7 +1022,9 @@
       <c r="L7" s="7">
         <v>135.81</v>
       </c>
-      <c r="M7" s="7"/>
+      <c r="M7" s="7">
+        <v>135.81</v>
+      </c>
       <c r="N7" s="7">
         <v>1</v>
       </c>
@@ -1039,7 +1059,9 @@
       <c r="E8" s="3">
         <v>1.3</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <v>1.3</v>
+      </c>
       <c r="G8" s="3">
         <v>1</v>
       </c>
@@ -1056,7 +1078,9 @@
       <c r="L8" s="7">
         <v>9.3699999999999992</v>
       </c>
-      <c r="M8" s="7"/>
+      <c r="M8" s="7">
+        <v>9.3699999999999992</v>
+      </c>
       <c r="N8" s="7">
         <v>1</v>
       </c>
@@ -1091,7 +1115,10 @@
       <c r="E9" s="3">
         <v>36000</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <f>13436+1133+58+2+2</f>
+        <v>14631</v>
+      </c>
       <c r="G9" s="3">
         <v>6</v>
       </c>
@@ -1144,7 +1171,10 @@
       <c r="E10" s="3">
         <v>36000</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <f>5726+556+36+2+2</f>
+        <v>6322</v>
+      </c>
       <c r="G10" s="3">
         <v>5</v>
       </c>
@@ -1197,7 +1227,10 @@
       <c r="E11" s="3">
         <v>36000</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3">
+        <f>13852+3644+800+129+14+1+2</f>
+        <v>18442</v>
+      </c>
       <c r="G11" s="3">
         <v>7</v>
       </c>
@@ -1250,7 +1283,9 @@
       <c r="E12" s="3">
         <v>36000</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3">
+        <v>35973</v>
+      </c>
       <c r="G12" s="3">
         <v>37</v>
       </c>
@@ -1264,8 +1299,8 @@
         <v>11409</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12" s="7" t="s">
-        <v>52</v>
+      <c r="L12" s="7">
+        <v>2316</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7">
@@ -1300,10 +1335,12 @@
         <v>32848</v>
       </c>
       <c r="E13" s="3">
+        <v>36000</v>
+      </c>
+      <c r="F13" s="3">
         <f>7132+269+5+2</f>
         <v>7408</v>
       </c>
-      <c r="F13" s="3"/>
       <c r="G13" s="3">
         <v>4</v>
       </c>
@@ -1354,10 +1391,11 @@
         <v>33486</v>
       </c>
       <c r="E14" s="3">
-        <f>2555+122+3</f>
+        <v>36000</v>
+      </c>
+      <c r="F14" s="3">
         <v>2680</v>
       </c>
-      <c r="F14" s="3"/>
       <c r="G14" s="3">
         <v>4</v>
       </c>
@@ -1408,10 +1446,12 @@
         <v>35309</v>
       </c>
       <c r="E15" s="3">
-        <f>42652+6711+789+61</f>
-        <v>50213</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>36000</v>
+      </c>
+      <c r="F15" s="3">
+        <f>30590+4706+534+42+2</f>
+        <v>35874</v>
+      </c>
       <c r="G15" s="3">
         <v>6</v>
       </c>
@@ -1462,10 +1502,12 @@
         <v>44497</v>
       </c>
       <c r="E16" s="3">
-        <f>18221+15023+11136+7400+4310+2163+900+298+73+11</f>
-        <v>59535</v>
-      </c>
-      <c r="F16" s="3"/>
+        <v>36000</v>
+      </c>
+      <c r="F16" s="3">
+        <f>10943+7877+5251+3042+1511+625+209+51+8+1+1</f>
+        <v>29519</v>
+      </c>
       <c r="G16" s="3">
         <v>11</v>
       </c>
@@ -1896,7 +1938,9 @@
       <c r="E24" s="3">
         <v>4470</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3">
+        <v>4470</v>
+      </c>
       <c r="G24" s="3">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Fill last update of LB
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F1D277-7D82-4740-8593-8A6A95F57F62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4959AB4-0711-4527-86A3-2FE01175A9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5720B9E1-D7F9-47BD-8756-C09FD62EA93D}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +627,7 @@
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
@@ -962,8 +962,7 @@
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="7">
-        <f>8591+1106+203+33+6+65</f>
-        <v>10004</v>
+        <v>36000</v>
       </c>
       <c r="M6" s="7">
         <f>8591+1106+203+33+6+65</f>
@@ -1133,10 +1132,12 @@
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M9" s="7">
         <f>11248+2596+178+13+69</f>
         <v>14104</v>
       </c>
-      <c r="M9" s="7"/>
       <c r="N9" s="7">
         <v>16</v>
       </c>
@@ -1189,10 +1190,12 @@
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M10" s="7">
         <f>11740+960+87+7+52</f>
         <v>12846</v>
       </c>
-      <c r="M10" s="7"/>
       <c r="N10" s="7">
         <v>16</v>
       </c>
@@ -1245,10 +1248,12 @@
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M11" s="7">
         <f>4680+743+148+25+6+39</f>
         <v>5641</v>
       </c>
-      <c r="M11" s="7"/>
       <c r="N11" s="7">
         <v>16</v>
       </c>
@@ -1302,7 +1307,9 @@
       <c r="L12" s="7">
         <v>2316</v>
       </c>
-      <c r="M12" s="7"/>
+      <c r="M12" s="7">
+        <v>2316</v>
+      </c>
       <c r="N12" s="7">
         <v>36</v>
       </c>
@@ -1355,10 +1362,12 @@
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M13" s="7">
         <f>14452+647+31+119</f>
         <v>15249</v>
       </c>
-      <c r="M13" s="7"/>
       <c r="N13" s="7">
         <v>16</v>
       </c>
@@ -1410,10 +1419,12 @@
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M14" s="7">
         <f>7279+375+25+114</f>
         <v>7793</v>
       </c>
-      <c r="M14" s="7"/>
       <c r="N14" s="7">
         <v>16</v>
       </c>
@@ -1466,10 +1477,12 @@
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M15" s="7">
         <f>6562+754+81+14+56</f>
         <v>7467</v>
       </c>
-      <c r="M15" s="7"/>
       <c r="N15" s="7">
         <v>16</v>
       </c>
@@ -1522,10 +1535,11 @@
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="7">
-        <f>4978+4134+2857+2348+1799+1402+1020+916+807+1079+1401+2153+2346+1912+1547+1084+873+710+777+782+1133+1250+1655+1428+1331+826+514+260+117+47+19+8+6+28</f>
-        <v>43547</v>
-      </c>
-      <c r="M16" s="7"/>
+        <v>36000</v>
+      </c>
+      <c r="M16" s="7">
+        <v>31735</v>
+      </c>
       <c r="N16" s="7">
         <v>36</v>
       </c>
@@ -1558,10 +1572,11 @@
         <v>33320</v>
       </c>
       <c r="E17" s="3">
-        <f>50558+1348+18</f>
+        <v>72000</v>
+      </c>
+      <c r="F17" s="3">
         <v>51924</v>
       </c>
-      <c r="F17" s="3"/>
       <c r="G17" s="3">
         <v>4</v>
       </c>
@@ -1576,10 +1591,12 @@
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M17" s="7">
         <f>4405+119+350</f>
         <v>4874</v>
       </c>
-      <c r="M17" s="7"/>
       <c r="N17" s="7">
         <v>16</v>
       </c>
@@ -1612,10 +1629,12 @@
         <v>35321</v>
       </c>
       <c r="E18" s="3">
+        <v>72000</v>
+      </c>
+      <c r="F18" s="3">
         <f>24942+815+13</f>
         <v>25770</v>
       </c>
-      <c r="F18" s="3"/>
       <c r="G18" s="3">
         <v>4</v>
       </c>
@@ -1630,10 +1649,12 @@
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M18" s="7">
         <f>2173+86+301</f>
         <v>2560</v>
       </c>
-      <c r="M18" s="7"/>
       <c r="N18" s="7">
         <v>16</v>
       </c>
@@ -1666,10 +1687,12 @@
         <v>41340</v>
       </c>
       <c r="E19" s="3">
+        <v>72000</v>
+      </c>
+      <c r="F19" s="3">
         <f>28940+2746+170+6</f>
         <v>31862</v>
       </c>
-      <c r="F19" s="3"/>
       <c r="G19" s="3">
         <v>5</v>
       </c>
@@ -1684,10 +1707,12 @@
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M19" s="7">
         <f>2723+258+31+124</f>
         <v>3136</v>
       </c>
-      <c r="M19" s="7"/>
       <c r="N19" s="7">
         <v>16</v>
       </c>
@@ -1720,10 +1745,12 @@
         <v>62818</v>
       </c>
       <c r="E20" s="3">
+        <v>72000</v>
+      </c>
+      <c r="F20" s="3">
         <f>32570+8971+2042+349+40+3</f>
         <v>43975</v>
       </c>
-      <c r="F20" s="3"/>
       <c r="G20" s="3">
         <v>7</v>
       </c>
@@ -1738,10 +1765,12 @@
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M20" s="7">
         <f>19275+3421+743+168+3512+55</f>
         <v>27174</v>
       </c>
-      <c r="M20" s="7"/>
       <c r="N20" s="7">
         <v>16</v>
       </c>
@@ -1774,10 +1803,12 @@
         <v>22545</v>
       </c>
       <c r="E21" s="3">
+        <v>36000</v>
+      </c>
+      <c r="F21" s="3">
         <f>5164+498+33+1</f>
         <v>5696</v>
       </c>
-      <c r="F21" s="3"/>
       <c r="G21" s="3">
         <v>5</v>
       </c>
@@ -1792,10 +1823,12 @@
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="7">
-        <f>6083+412+40+5+55</f>
-        <v>6595</v>
-      </c>
-      <c r="M21" s="7"/>
+        <v>36000</v>
+      </c>
+      <c r="M21" s="7">
+        <f>12245+895+79+7+55</f>
+        <v>13281</v>
+      </c>
       <c r="N21" s="7">
         <v>36</v>
       </c>
@@ -1828,10 +1861,12 @@
         <v>22841</v>
       </c>
       <c r="E22" s="3">
+        <v>36000</v>
+      </c>
+      <c r="F22" s="3">
         <f>8482+1495+192+17</f>
         <v>10186</v>
       </c>
-      <c r="F22" s="3"/>
       <c r="G22" s="3">
         <v>6</v>
       </c>
@@ -1846,10 +1881,12 @@
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="7">
-        <f>11046+798+106+16+4+38</f>
-        <v>12008</v>
-      </c>
-      <c r="M22" s="7"/>
+        <v>36000</v>
+      </c>
+      <c r="M22" s="7">
+        <f>23718+1715+237+32+6+39</f>
+        <v>25747</v>
+      </c>
       <c r="N22" s="7">
         <v>36</v>
       </c>
@@ -1882,10 +1919,12 @@
         <v>23122</v>
       </c>
       <c r="E23" s="3">
-        <f>7476+2800+887+239+48+7</f>
-        <v>11457</v>
-      </c>
-      <c r="F23" s="3"/>
+        <v>36000</v>
+      </c>
+      <c r="F23" s="3">
+        <f>13169+5437+2046+651+179+36+5+1</f>
+        <v>21524</v>
+      </c>
       <c r="G23" s="3">
         <v>9</v>
       </c>
@@ -1900,10 +1939,12 @@
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="7">
-        <f>4910+1142+256+71+21+7+3+25</f>
-        <v>6435</v>
-      </c>
-      <c r="M23" s="7"/>
+        <v>36000</v>
+      </c>
+      <c r="M23" s="7">
+        <f>8133+2217+507+137+42+13+4+25</f>
+        <v>11078</v>
+      </c>
       <c r="N23" s="7">
         <v>36</v>
       </c>
@@ -1959,7 +2000,9 @@
       <c r="L24" s="7">
         <v>333.02</v>
       </c>
-      <c r="M24" s="7"/>
+      <c r="M24" s="7">
+        <v>333.02</v>
+      </c>
       <c r="N24" s="7">
         <v>36</v>
       </c>
@@ -1994,10 +2037,12 @@
         <v>1474</v>
       </c>
       <c r="E25" s="3">
+        <v>36000</v>
+      </c>
+      <c r="F25" s="3">
         <f>18100+645+12</f>
         <v>18757</v>
       </c>
-      <c r="F25" s="3"/>
       <c r="G25" s="3">
         <v>4</v>
       </c>
@@ -2012,10 +2057,12 @@
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M25" s="7">
         <f>1782+72+260</f>
         <v>2114</v>
       </c>
-      <c r="M25" s="7"/>
       <c r="N25" s="7">
         <v>16</v>
       </c>
@@ -2048,10 +2095,12 @@
         <v>232</v>
       </c>
       <c r="E26" s="3">
-        <f>7107+1428+224+24+1</f>
-        <v>8784</v>
-      </c>
-      <c r="F26" s="3"/>
+        <v>36000</v>
+      </c>
+      <c r="F26" s="3">
+        <f>19956+5074+1068+178+21+1+1</f>
+        <v>26299</v>
+      </c>
       <c r="G26" s="3">
         <v>7</v>
       </c>
@@ -2066,10 +2115,12 @@
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="7">
-        <f>47056+4159+438+77+13+4+47</f>
-        <v>51794</v>
-      </c>
-      <c r="M26" s="7"/>
+        <v>36000</v>
+      </c>
+      <c r="M26" s="7">
+        <f>6356+698+122+21+5+42</f>
+        <v>7244</v>
+      </c>
       <c r="N26" s="7">
         <v>36</v>
       </c>
@@ -2104,7 +2155,9 @@
       <c r="E27" s="3">
         <v>0.9</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3">
+        <v>0.9</v>
+      </c>
       <c r="G27" s="3">
         <v>1</v>
       </c>
@@ -2121,7 +2174,9 @@
       <c r="L27" s="7">
         <v>8.34</v>
       </c>
-      <c r="M27" s="7"/>
+      <c r="M27" s="7">
+        <v>8.34</v>
+      </c>
       <c r="N27" s="7">
         <v>1</v>
       </c>
@@ -2156,7 +2211,9 @@
       <c r="E28" s="3">
         <v>0.2</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3">
+        <v>0.2</v>
+      </c>
       <c r="G28" s="3">
         <v>1</v>
       </c>
@@ -2173,7 +2230,9 @@
       <c r="L28" s="7">
         <v>7.02</v>
       </c>
-      <c r="M28" s="7"/>
+      <c r="M28" s="7">
+        <v>7.02</v>
+      </c>
       <c r="N28" s="7">
         <v>1</v>
       </c>
@@ -2208,7 +2267,9 @@
       <c r="E29" s="3">
         <v>2407</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3">
+        <v>2407</v>
+      </c>
       <c r="G29" s="3">
         <v>50</v>
       </c>
@@ -2225,7 +2286,9 @@
       <c r="L29" s="7">
         <v>1225.27</v>
       </c>
-      <c r="M29" s="7"/>
+      <c r="M29" s="7">
+        <v>1225.27</v>
+      </c>
       <c r="N29" s="7">
         <v>16</v>
       </c>
@@ -2260,7 +2323,9 @@
       <c r="E30" s="3">
         <v>0.4</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3">
+        <v>0.4</v>
+      </c>
       <c r="G30" s="3">
         <v>1</v>
       </c>
@@ -2277,7 +2342,9 @@
       <c r="L30" s="7">
         <v>3005.15</v>
       </c>
-      <c r="M30" s="7"/>
+      <c r="M30" s="7">
+        <v>3005.15</v>
+      </c>
       <c r="N30" s="7">
         <v>16</v>
       </c>
@@ -2314,7 +2381,9 @@
       <c r="E31" s="3">
         <v>0.4</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3">
+        <v>0.4</v>
+      </c>
       <c r="G31" s="3">
         <v>1</v>
       </c>
@@ -2331,7 +2400,9 @@
       <c r="L31" s="7">
         <v>65.099999999999994</v>
       </c>
-      <c r="M31" s="7"/>
+      <c r="M31" s="7">
+        <v>65.099999999999994</v>
+      </c>
       <c r="N31" s="7">
         <v>1</v>
       </c>
@@ -2366,7 +2437,9 @@
       <c r="E32" s="3">
         <v>0.8</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3">
+        <v>0.8</v>
+      </c>
       <c r="G32" s="3">
         <v>1</v>
       </c>
@@ -2383,7 +2456,9 @@
       <c r="L32" s="7">
         <v>186.81</v>
       </c>
-      <c r="M32" s="7"/>
+      <c r="M32" s="7">
+        <v>186.81</v>
+      </c>
       <c r="N32" s="7">
         <v>1</v>
       </c>
@@ -2418,7 +2493,9 @@
       <c r="E33" s="3">
         <v>2</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3">
+        <v>2</v>
+      </c>
       <c r="G33" s="3">
         <v>1</v>
       </c>
@@ -2435,7 +2512,9 @@
       <c r="L33" s="7">
         <v>431.65</v>
       </c>
-      <c r="M33" s="7"/>
+      <c r="M33" s="7">
+        <v>431.65</v>
+      </c>
       <c r="N33" s="7">
         <v>1</v>
       </c>
@@ -2468,10 +2547,12 @@
         <v>2101</v>
       </c>
       <c r="E34" s="3">
+        <v>72000</v>
+      </c>
+      <c r="F34" s="3">
         <f>39404+12782+3093+464+44+7</f>
         <v>55794</v>
       </c>
-      <c r="F34" s="3"/>
       <c r="G34" s="3">
         <v>7</v>
       </c>
@@ -2486,10 +2567,12 @@
       </c>
       <c r="K34" s="3"/>
       <c r="L34" s="7">
-        <f>225+198+288</f>
-        <v>711</v>
-      </c>
-      <c r="M34" s="7"/>
+        <v>36000</v>
+      </c>
+      <c r="M34" s="7">
+        <f>254+194+283</f>
+        <v>731</v>
+      </c>
       <c r="N34" s="7">
         <v>16</v>
       </c>
@@ -2522,10 +2605,12 @@
         <v>2080</v>
       </c>
       <c r="E35" s="3">
+        <v>72000</v>
+      </c>
+      <c r="F35" s="3">
         <f>38573+12766+3355+563+40+7+15+7+3</f>
         <v>55329</v>
       </c>
-      <c r="F35" s="3"/>
       <c r="G35" s="3">
         <v>9</v>
       </c>
@@ -2540,10 +2625,12 @@
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M35" s="7">
         <f>328+321+333+438</f>
         <v>1420</v>
       </c>
-      <c r="M35" s="7"/>
       <c r="N35" s="7">
         <v>12</v>
       </c>
@@ -2576,10 +2663,12 @@
         <v>2307</v>
       </c>
       <c r="E36" s="3">
+        <v>72000</v>
+      </c>
+      <c r="F36" s="3">
         <f>18532+4458+724+50+11+17+8+3</f>
         <v>23803</v>
       </c>
-      <c r="F36" s="3"/>
       <c r="G36" s="3">
         <v>8</v>
       </c>
@@ -2594,10 +2683,12 @@
       </c>
       <c r="K36" s="3"/>
       <c r="L36" s="7">
-        <f>262+268+267+346</f>
-        <v>1143</v>
-      </c>
-      <c r="M36" s="7"/>
+        <v>36000</v>
+      </c>
+      <c r="M36" s="7">
+        <f>400+406+409+531</f>
+        <v>1746</v>
+      </c>
       <c r="N36" s="7">
         <v>11</v>
       </c>
@@ -2630,10 +2721,12 @@
         <v>13135</v>
       </c>
       <c r="E37" s="3">
+        <v>36000</v>
+      </c>
+      <c r="F37" s="3">
         <f>9463+869+51+2</f>
         <v>10385</v>
       </c>
-      <c r="F37" s="3"/>
       <c r="G37" s="3">
         <v>5</v>
       </c>
@@ -2648,10 +2741,12 @@
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M37" s="7">
         <f>28032+1690+128+12+65</f>
         <v>29927</v>
       </c>
-      <c r="M37" s="7"/>
       <c r="N37" s="7">
         <v>16</v>
       </c>
@@ -2684,10 +2779,12 @@
         <v>13802</v>
       </c>
       <c r="E38" s="3">
+        <v>36000</v>
+      </c>
+      <c r="F38" s="3">
         <f>15553+2465+281+20+2</f>
         <v>18321</v>
       </c>
-      <c r="F38" s="3"/>
       <c r="G38" s="3">
         <v>6</v>
       </c>
@@ -2702,10 +2799,12 @@
       </c>
       <c r="K38" s="3"/>
       <c r="L38" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M38" s="7">
         <f>3939+412+45+6+42</f>
         <v>4444</v>
       </c>
-      <c r="M38" s="7"/>
       <c r="N38" s="7">
         <v>16</v>
       </c>
@@ -2738,10 +2837,12 @@
         <v>16540</v>
       </c>
       <c r="E39" s="3">
+        <v>36000</v>
+      </c>
+      <c r="F39" s="3">
         <f>6822+1934+449+77+9+2</f>
         <v>9293</v>
       </c>
-      <c r="F39" s="3"/>
       <c r="G39" s="3">
         <v>7</v>
       </c>
@@ -2756,10 +2857,12 @@
       </c>
       <c r="K39" s="3"/>
       <c r="L39" s="7">
+        <v>36000</v>
+      </c>
+      <c r="M39" s="7">
         <f>7879+1078+180+38+9+5+34</f>
         <v>9223</v>
       </c>
-      <c r="M39" s="7"/>
       <c r="N39" s="7">
         <v>36</v>
       </c>
@@ -2794,7 +2897,9 @@
       <c r="E40" s="3">
         <v>18677</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3">
+        <v>18677</v>
+      </c>
       <c r="G40" s="3">
         <v>40</v>
       </c>
@@ -2811,7 +2916,9 @@
       <c r="L40" s="7">
         <v>1433.11</v>
       </c>
-      <c r="M40" s="7"/>
+      <c r="M40" s="7">
+        <v>1433.11</v>
+      </c>
       <c r="N40" s="7">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Cut 20h to 10h
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4959AB4-0711-4527-86A3-2FE01175A9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2DCD7D-6427-45E4-94EA-623D6B085F65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="53">
   <si>
     <t>Sample</t>
   </si>
@@ -617,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5720B9E1-D7F9-47BD-8756-C09FD62EA93D}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,23 +941,23 @@
         <v>1399</v>
       </c>
       <c r="E6" s="3">
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="F6" s="3">
-        <f>51178+14426+3116+440+35+1+1</f>
-        <v>69197</v>
+        <v>18020</v>
       </c>
       <c r="G6" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>49</v>
       </c>
       <c r="I6" s="12">
-        <v>0.42609582059123341</v>
+        <f>(D6-J6)/J6</f>
+        <v>0.42755102040816328</v>
       </c>
       <c r="J6" s="3">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="7">
@@ -1528,6 +1527,7 @@
         <v>49</v>
       </c>
       <c r="I16" s="12">
+        <f>(D16-J16)/J16</f>
         <v>0.14127061478878658</v>
       </c>
       <c r="J16" s="3">
@@ -1550,6 +1550,7 @@
         <v>49</v>
       </c>
       <c r="Q16" s="8">
+        <f>(D16-R16)/R16</f>
         <v>6.8611911623439006E-2</v>
       </c>
       <c r="R16" s="7">
@@ -1572,22 +1573,24 @@
         <v>33320</v>
       </c>
       <c r="E17" s="3">
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="F17" s="3">
-        <v>51924</v>
+        <f>1+18+348</f>
+        <v>367</v>
       </c>
       <c r="G17" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>49</v>
       </c>
       <c r="I17" s="12">
-        <v>0.19242744157749705</v>
+        <f>(D17-J17)/J17</f>
+        <v>0.1955936703864509</v>
       </c>
       <c r="J17" s="3">
-        <v>27943</v>
+        <v>27869</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="7">
@@ -1629,11 +1632,10 @@
         <v>35321</v>
       </c>
       <c r="E18" s="3">
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="F18" s="3">
-        <f>24942+815+13</f>
-        <v>25770</v>
+        <v>25773</v>
       </c>
       <c r="G18" s="3">
         <v>4</v>
@@ -1642,6 +1644,7 @@
         <v>49</v>
       </c>
       <c r="I18" s="12">
+        <f>(D18-J18)/J18</f>
         <v>0.25451962351269758</v>
       </c>
       <c r="J18" s="3">
@@ -1687,11 +1690,10 @@
         <v>41340</v>
       </c>
       <c r="E19" s="3">
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="F19" s="3">
-        <f>28940+2746+170+6</f>
-        <v>31862</v>
+        <v>31863</v>
       </c>
       <c r="G19" s="3">
         <v>5</v>
@@ -1745,23 +1747,23 @@
         <v>62818</v>
       </c>
       <c r="E20" s="3">
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="F20" s="3">
-        <f>32570+8971+2042+349+40+3</f>
-        <v>43975</v>
+        <v>11405</v>
       </c>
       <c r="G20" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>49</v>
       </c>
       <c r="I20" s="12">
-        <v>0.63724979149291072</v>
+        <f>(D20-J20)/J20</f>
+        <v>0.64716679340273231</v>
       </c>
       <c r="J20" s="3">
-        <v>38368</v>
+        <v>38137</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="7">
@@ -2547,14 +2549,13 @@
         <v>2101</v>
       </c>
       <c r="E34" s="3">
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="F34" s="3">
-        <f>39404+12782+3093+464+44+7</f>
-        <v>55794</v>
+        <v>16392</v>
       </c>
       <c r="G34" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>49</v>
@@ -2605,14 +2606,13 @@
         <v>2080</v>
       </c>
       <c r="E35" s="3">
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="F35" s="3">
-        <f>38573+12766+3355+563+40+7+15+7+3</f>
-        <v>55329</v>
+        <v>16757</v>
       </c>
       <c r="G35" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>49</v>
@@ -2663,7 +2663,7 @@
         <v>2307</v>
       </c>
       <c r="E36" s="3">
-        <v>72000</v>
+        <v>36000</v>
       </c>
       <c r="F36" s="3">
         <f>18532+4458+724+50+11+17+8+3</f>
@@ -2941,334 +2941,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7928A525-2596-480E-B92E-D5374D261C54}">
-  <dimension ref="A1:B39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="A1:B39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1390</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>14832</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>6207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>6653</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>8446</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>11822</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>32848</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>33486</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>35309</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>44497</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>33320</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>35321</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>41340</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>62818</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>22545</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>22841</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>23122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23">
-        <v>66857</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>1474</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>1644</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
-        <v>2376</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32">
-        <v>2547</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33">
-        <v>2101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34">
-        <v>2080</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35">
-        <v>2307</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36">
-        <v>13135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37">
-        <v>13802</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38">
-        <v>16540</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39">
-        <v>25977</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B39">
-    <sortCondition ref="A5"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Measure just first layer for DP
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2DCD7D-6427-45E4-94EA-623D6B085F65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA73CD0C-A304-4794-ACF3-9DD64512D44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
@@ -617,7 +617,7 @@
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,16 +1018,16 @@
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="7">
-        <v>135.81</v>
+        <v>0.52</v>
       </c>
       <c r="M7" s="7">
-        <v>135.81</v>
+        <v>0.52</v>
       </c>
       <c r="N7" s="7">
         <v>1</v>
       </c>
       <c r="O7" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>48</v>
@@ -1074,16 +1074,16 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="7">
-        <v>9.3699999999999992</v>
+        <v>0.68</v>
       </c>
       <c r="M8" s="7">
-        <v>9.3699999999999992</v>
+        <v>0.68</v>
       </c>
       <c r="N8" s="7">
         <v>1</v>
       </c>
       <c r="O8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>48</v>
@@ -2174,16 +2174,17 @@
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="7">
-        <v>8.34</v>
+        <v>0.25</v>
       </c>
       <c r="M27" s="7">
-        <v>8.34</v>
+        <f>L27</f>
+        <v>0.25</v>
       </c>
       <c r="N27" s="7">
         <v>1</v>
       </c>
       <c r="O27" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P27" s="10" t="s">
         <v>48</v>
@@ -2230,16 +2231,17 @@
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="7">
-        <v>7.02</v>
+        <v>0.25</v>
       </c>
       <c r="M28" s="7">
-        <v>7.02</v>
+        <f>L28</f>
+        <v>0.25</v>
       </c>
       <c r="N28" s="7">
         <v>1</v>
       </c>
       <c r="O28" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P28" s="10" t="s">
         <v>48</v>
@@ -2400,16 +2402,17 @@
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="7">
-        <v>65.099999999999994</v>
+        <v>0.67</v>
       </c>
       <c r="M31" s="7">
-        <v>65.099999999999994</v>
+        <f>L31</f>
+        <v>0.67</v>
       </c>
       <c r="N31" s="7">
         <v>1</v>
       </c>
       <c r="O31" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P31" s="10" t="s">
         <v>48</v>
@@ -2456,16 +2459,17 @@
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="7">
-        <v>186.81</v>
+        <v>1.42</v>
       </c>
       <c r="M32" s="7">
-        <v>186.81</v>
+        <f>L32</f>
+        <v>1.42</v>
       </c>
       <c r="N32" s="7">
         <v>1</v>
       </c>
       <c r="O32" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P32" s="10" t="s">
         <v>48</v>
@@ -2512,16 +2516,17 @@
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="7">
-        <v>431.65</v>
+        <v>3.59</v>
       </c>
       <c r="M33" s="7">
-        <v>431.65</v>
+        <f>L33</f>
+        <v>3.59</v>
       </c>
       <c r="N33" s="7">
         <v>1</v>
       </c>
       <c r="O33" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P33" s="10" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Cut exact solutions with gap 5%
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -1,32 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stas\Documents\repo\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA73CD0C-A304-4794-ACF3-9DD64512D44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F4642A-083E-48E7-BEEE-88E9044CAFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -198,6 +190,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -269,11 +264,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,10 +295,12 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Процентный" xfId="1" builtinId="5"/>
+    <cellStyle name="Финансовый" xfId="2" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -617,7 +615,7 @@
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,6 +636,7 @@
     <col min="16" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1285,44 +1284,48 @@
         <v>11822</v>
       </c>
       <c r="E12" s="3">
-        <v>36000</v>
+        <v>35865</v>
       </c>
       <c r="F12" s="3">
-        <v>35973</v>
+        <f>E12</f>
+        <v>35865</v>
       </c>
       <c r="G12" s="3">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>49</v>
       </c>
       <c r="I12" s="12">
-        <v>3.6199491629415374E-2</v>
+        <f>(D12-J12)/J12</f>
+        <v>4.8607415291821894E-2</v>
       </c>
       <c r="J12" s="3">
-        <v>11409</v>
+        <v>11274</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="7">
-        <v>2316</v>
+        <v>2225</v>
       </c>
       <c r="M12" s="7">
-        <v>2316</v>
+        <f>L12</f>
+        <v>2225</v>
       </c>
       <c r="N12" s="7">
         <v>36</v>
       </c>
       <c r="O12" s="7">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q12" s="8">
-        <v>2.5382858109823165E-4</v>
+        <f>(D12-R12)/R12</f>
+        <v>4.7121346324180691E-2</v>
       </c>
       <c r="R12" s="7">
-        <v>11819</v>
+        <v>11290</v>
       </c>
       <c r="S12" s="7"/>
       <c r="U12" s="11"/>
@@ -2288,28 +2291,30 @@
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="7">
-        <v>1225.27</v>
+        <v>682</v>
       </c>
       <c r="M29" s="7">
-        <v>1225.27</v>
+        <f>L29</f>
+        <v>682</v>
       </c>
       <c r="N29" s="7">
         <v>16</v>
       </c>
       <c r="O29" s="7">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="P29" s="10" t="s">
         <v>48</v>
       </c>
       <c r="Q29" s="8">
-        <v>0</v>
+        <f>(D29-R29)/R29</f>
+        <v>4.8207663782447466E-2</v>
       </c>
       <c r="R29" s="7">
-        <v>848</v>
+        <v>809</v>
       </c>
       <c r="S29" s="7"/>
-      <c r="U29" s="11"/>
+      <c r="U29" s="13"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -2344,30 +2349,30 @@
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="7">
-        <v>3005.15</v>
+        <v>0.53</v>
       </c>
       <c r="M30" s="7">
-        <v>3005.15</v>
+        <f>L30</f>
+        <v>0.53</v>
       </c>
       <c r="N30" s="7">
         <v>16</v>
       </c>
       <c r="O30" s="7">
-        <v>151</v>
+        <v>1</v>
       </c>
       <c r="P30" s="10" t="s">
         <v>48</v>
       </c>
       <c r="Q30" s="8">
-        <v>0</v>
+        <f>(D30-R30)/R30</f>
+        <v>4.5824094604582408E-2</v>
       </c>
       <c r="R30" s="7">
-        <v>1414</v>
-      </c>
-      <c r="S30" s="7">
-        <v>1414</v>
-      </c>
-      <c r="U30" s="11"/>
+        <v>1353</v>
+      </c>
+      <c r="S30" s="7"/>
+      <c r="U30" s="13"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -2919,25 +2924,27 @@
       </c>
       <c r="K40" s="3"/>
       <c r="L40" s="7">
-        <v>1433.11</v>
+        <v>1401</v>
       </c>
       <c r="M40" s="7">
-        <v>1433.11</v>
+        <f>L40</f>
+        <v>1401</v>
       </c>
       <c r="N40" s="7">
         <v>16</v>
       </c>
       <c r="O40" s="7">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="P40" s="10" t="s">
         <v>48</v>
       </c>
       <c r="Q40" s="8">
-        <v>0</v>
+        <f>(D40-R40)/R40</f>
+        <v>3.7295851136045999E-2</v>
       </c>
       <c r="R40" s="7">
-        <v>25977</v>
+        <v>25043</v>
       </c>
       <c r="S40" s="7"/>
       <c r="U40" s="11"/>

</xml_diff>

<commit_message>
Add main table for Optima's paper
</commit_message>
<xml_diff>
--- a/playground/report/salman.xlsx
+++ b/playground/report/salman.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stas\Documents\repo\pcgtsp-bnb\playground\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\pcgtsp-bnb\playground\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F4642A-083E-48E7-BEEE-88E9044CAFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D85F629-740A-4024-B418-A839A835378B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7907F53B-C8ED-4F7C-8267-210B91F70DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Оптима" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="61">
   <si>
     <t>Sample</t>
   </si>
@@ -184,6 +193,30 @@
   </si>
   <si>
     <t>LastLB</t>
+  </si>
+  <si>
+    <t>Instance</t>
+  </si>
+  <si>
+    <t>Gurobi</t>
+  </si>
+  <si>
+    <t>Branch &amp; Bound</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -193,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +245,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -240,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -263,13 +305,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,6 +375,30 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -614,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5720B9E1-D7F9-47BD-8756-C09FD62EA93D}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,7 +2283,7 @@
         <v>0.25</v>
       </c>
       <c r="M27" s="7">
-        <f>L27</f>
+        <f t="shared" ref="M27:M33" si="0">L27</f>
         <v>0.25</v>
       </c>
       <c r="N27" s="7">
@@ -2237,7 +2340,7 @@
         <v>0.25</v>
       </c>
       <c r="M28" s="7">
-        <f>L28</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="N28" s="7">
@@ -2294,7 +2397,7 @@
         <v>682</v>
       </c>
       <c r="M29" s="7">
-        <f>L29</f>
+        <f t="shared" si="0"/>
         <v>682</v>
       </c>
       <c r="N29" s="7">
@@ -2352,7 +2455,7 @@
         <v>0.53</v>
       </c>
       <c r="M30" s="7">
-        <f>L30</f>
+        <f t="shared" si="0"/>
         <v>0.53</v>
       </c>
       <c r="N30" s="7">
@@ -2410,7 +2513,7 @@
         <v>0.67</v>
       </c>
       <c r="M31" s="7">
-        <f>L31</f>
+        <f t="shared" si="0"/>
         <v>0.67</v>
       </c>
       <c r="N31" s="7">
@@ -2467,7 +2570,7 @@
         <v>1.42</v>
       </c>
       <c r="M32" s="7">
-        <f>L32</f>
+        <f t="shared" si="0"/>
         <v>1.42</v>
       </c>
       <c r="N32" s="7">
@@ -2524,7 +2627,7 @@
         <v>3.59</v>
       </c>
       <c r="M33" s="7">
-        <f>L33</f>
+        <f t="shared" si="0"/>
         <v>3.59</v>
       </c>
       <c r="N33" s="7">
@@ -2953,4 +3056,1822 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBE960C-C4EF-4AB2-A07F-63C1D9F34223}">
+  <dimension ref="A1:T41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="11"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>92</v>
+      </c>
+      <c r="D3" s="5">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5">
+        <v>43</v>
+      </c>
+      <c r="F3" s="5">
+        <v>107.28</v>
+      </c>
+      <c r="G3" s="5">
+        <v>43</v>
+      </c>
+      <c r="H3" s="20">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="J3" s="5">
+        <v>43</v>
+      </c>
+      <c r="K3" s="20">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>27.3</v>
+      </c>
+      <c r="M3" s="5">
+        <v>43</v>
+      </c>
+      <c r="N3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>39</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1730</v>
+      </c>
+      <c r="F4" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1730</v>
+      </c>
+      <c r="H4" s="20">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1726</v>
+      </c>
+      <c r="K4" s="20">
+        <v>2.3174971031286211E-3</v>
+      </c>
+      <c r="L4" s="5">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1730</v>
+      </c>
+      <c r="N4" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>65</v>
+      </c>
+      <c r="D5" s="5">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1390</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1390</v>
+      </c>
+      <c r="H5" s="20">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="J5" s="5">
+        <v>1385</v>
+      </c>
+      <c r="K5" s="20">
+        <v>3.6101083032490976E-3</v>
+      </c>
+      <c r="L5" s="5">
+        <v>14.99</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1390</v>
+      </c>
+      <c r="N5" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>133</v>
+      </c>
+      <c r="D6" s="5">
+        <v>26</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1418</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4.45</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1383</v>
+      </c>
+      <c r="H6" s="20">
+        <v>2.5307302964569775E-2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>32</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1383</v>
+      </c>
+      <c r="K6" s="20">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>60.69</v>
+      </c>
+      <c r="M6" s="5">
+        <v>1383</v>
+      </c>
+      <c r="N6" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>244</v>
+      </c>
+      <c r="D7" s="5">
+        <v>48</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1399</v>
+      </c>
+      <c r="F7" s="5">
+        <v>52.01</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1063</v>
+      </c>
+      <c r="H7" s="20">
+        <v>0.3160865475070555</v>
+      </c>
+      <c r="I7" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J7" s="5">
+        <v>980</v>
+      </c>
+      <c r="K7" s="20">
+        <v>0.42755102040816328</v>
+      </c>
+      <c r="L7" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M7" s="5">
+        <v>981</v>
+      </c>
+      <c r="N7" s="20">
+        <v>0.42609582059123341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>349</v>
+      </c>
+      <c r="D8" s="5">
+        <v>64</v>
+      </c>
+      <c r="E8" s="5">
+        <v>62</v>
+      </c>
+      <c r="F8" s="5">
+        <v>380.65</v>
+      </c>
+      <c r="G8" s="5">
+        <v>62</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="J8" s="5">
+        <v>62</v>
+      </c>
+      <c r="K8" s="20">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="M8" s="5">
+        <v>62</v>
+      </c>
+      <c r="N8" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5">
+        <v>414</v>
+      </c>
+      <c r="D9" s="5">
+        <v>79</v>
+      </c>
+      <c r="E9" s="5">
+        <v>14832</v>
+      </c>
+      <c r="F9" s="5">
+        <v>43200.01</v>
+      </c>
+      <c r="G9" s="5">
+        <v>14581</v>
+      </c>
+      <c r="H9" s="20">
+        <v>1.721418284068308E-2</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="J9" s="5">
+        <v>14594</v>
+      </c>
+      <c r="K9" s="20">
+        <v>1.6308071810333013E-2</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="M9" s="5">
+        <v>14594</v>
+      </c>
+      <c r="N9" s="20">
+        <v>1.6308071810333013E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>281</v>
+      </c>
+      <c r="D10" s="5">
+        <v>53</v>
+      </c>
+      <c r="E10" s="5">
+        <v>6207</v>
+      </c>
+      <c r="F10" s="5">
+        <v>42099</v>
+      </c>
+      <c r="G10" s="5">
+        <v>6022</v>
+      </c>
+      <c r="H10" s="20">
+        <v>2.9558286283626702E-2</v>
+      </c>
+      <c r="I10" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J10" s="5">
+        <v>4839</v>
+      </c>
+      <c r="K10" s="20">
+        <v>0.28270303781773093</v>
+      </c>
+      <c r="L10" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M10" s="5">
+        <v>4839</v>
+      </c>
+      <c r="N10" s="20">
+        <v>0.28270303781773093</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5">
+        <v>274</v>
+      </c>
+      <c r="D11" s="5">
+        <v>53</v>
+      </c>
+      <c r="E11" s="5">
+        <v>6653</v>
+      </c>
+      <c r="F11" s="5">
+        <v>42137</v>
+      </c>
+      <c r="G11" s="5">
+        <v>6184</v>
+      </c>
+      <c r="H11" s="20">
+        <v>7.5840879689521343E-2</v>
+      </c>
+      <c r="I11" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J11" s="5">
+        <v>4934</v>
+      </c>
+      <c r="K11" s="20">
+        <v>0.3483988650182408</v>
+      </c>
+      <c r="L11" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M11" s="5">
+        <v>4940</v>
+      </c>
+      <c r="N11" s="20">
+        <v>0.34676113360323885</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5">
+        <v>281</v>
+      </c>
+      <c r="D12" s="5">
+        <v>53</v>
+      </c>
+      <c r="E12" s="5">
+        <v>8446</v>
+      </c>
+      <c r="F12" s="5">
+        <v>42194</v>
+      </c>
+      <c r="G12" s="5">
+        <v>6936</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0.21770472895040369</v>
+      </c>
+      <c r="I12" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J12" s="5">
+        <v>5465</v>
+      </c>
+      <c r="K12" s="20">
+        <v>0.54547118023787744</v>
+      </c>
+      <c r="L12" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M12" s="5">
+        <v>5465</v>
+      </c>
+      <c r="N12" s="20">
+        <v>0.54547118023787744</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5">
+        <v>275</v>
+      </c>
+      <c r="D13" s="5">
+        <v>53</v>
+      </c>
+      <c r="E13" s="5">
+        <v>11822</v>
+      </c>
+      <c r="F13" s="5">
+        <v>23238.81</v>
+      </c>
+      <c r="G13" s="5">
+        <v>11822</v>
+      </c>
+      <c r="H13" s="20">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>35865</v>
+      </c>
+      <c r="J13" s="5">
+        <v>11274</v>
+      </c>
+      <c r="K13" s="20">
+        <v>4.8607415291821894E-2</v>
+      </c>
+      <c r="L13" s="5">
+        <v>2225</v>
+      </c>
+      <c r="M13" s="5">
+        <v>11290</v>
+      </c>
+      <c r="N13" s="20">
+        <v>4.7121346324180691E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5">
+        <v>346</v>
+      </c>
+      <c r="D14" s="5">
+        <v>70</v>
+      </c>
+      <c r="E14" s="5">
+        <v>32848</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J14" s="5">
+        <v>31153</v>
+      </c>
+      <c r="K14" s="20">
+        <v>5.4408885179597473E-2</v>
+      </c>
+      <c r="L14" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M14" s="5">
+        <v>31177</v>
+      </c>
+      <c r="N14" s="20">
+        <v>5.3597203066363022E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="5">
+        <v>351</v>
+      </c>
+      <c r="D15" s="5">
+        <v>70</v>
+      </c>
+      <c r="E15" s="5">
+        <v>33486</v>
+      </c>
+      <c r="F15" s="5">
+        <v>42021</v>
+      </c>
+      <c r="G15" s="5">
+        <v>31840</v>
+      </c>
+      <c r="H15" s="20">
+        <v>5.0502512562814073E-2</v>
+      </c>
+      <c r="I15" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J15" s="5">
+        <v>31268</v>
+      </c>
+      <c r="K15" s="20">
+        <v>7.0935141358577453E-2</v>
+      </c>
+      <c r="L15" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M15" s="5">
+        <v>31273</v>
+      </c>
+      <c r="N15" s="20">
+        <v>7.0763917756531194E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5">
+        <v>347</v>
+      </c>
+      <c r="D16" s="5">
+        <v>70</v>
+      </c>
+      <c r="E16" s="5">
+        <v>35309</v>
+      </c>
+      <c r="F16" s="5">
+        <v>41173</v>
+      </c>
+      <c r="G16" s="5">
+        <v>32944</v>
+      </c>
+      <c r="H16" s="20">
+        <v>7.1788489558037877E-2</v>
+      </c>
+      <c r="I16" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J16" s="5">
+        <v>32180</v>
+      </c>
+      <c r="K16" s="20">
+        <v>9.7234307022995653E-2</v>
+      </c>
+      <c r="L16" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M16" s="5">
+        <v>32180</v>
+      </c>
+      <c r="N16" s="20">
+        <v>9.7234307022995653E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="5">
+        <v>353</v>
+      </c>
+      <c r="D17" s="5">
+        <v>70</v>
+      </c>
+      <c r="E17" s="5">
+        <v>44497</v>
+      </c>
+      <c r="F17" s="5">
+        <v>41827</v>
+      </c>
+      <c r="G17" s="5">
+        <v>41378</v>
+      </c>
+      <c r="H17" s="20">
+        <v>7.5257383150466428E-2</v>
+      </c>
+      <c r="I17" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J17" s="5">
+        <v>38989</v>
+      </c>
+      <c r="K17" s="20">
+        <v>0.14127061478878658</v>
+      </c>
+      <c r="L17" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M17" s="5">
+        <v>41640</v>
+      </c>
+      <c r="N17" s="20">
+        <v>6.8611911623439006E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5">
+        <v>514</v>
+      </c>
+      <c r="D18" s="5">
+        <v>100</v>
+      </c>
+      <c r="E18" s="5">
+        <v>33320</v>
+      </c>
+      <c r="F18" s="5">
+        <v>34162</v>
+      </c>
+      <c r="G18" s="5">
+        <v>29926</v>
+      </c>
+      <c r="H18" s="20">
+        <v>0.11341308561117423</v>
+      </c>
+      <c r="I18" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J18" s="5">
+        <v>27869</v>
+      </c>
+      <c r="K18" s="20">
+        <v>0.1955936703864509</v>
+      </c>
+      <c r="L18" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M18" s="5">
+        <v>27943</v>
+      </c>
+      <c r="N18" s="20">
+        <v>0.19242744157749705</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5">
+        <v>524</v>
+      </c>
+      <c r="D19" s="5">
+        <v>100</v>
+      </c>
+      <c r="E19" s="5">
+        <v>35321</v>
+      </c>
+      <c r="F19" s="5">
+        <v>35379</v>
+      </c>
+      <c r="G19" s="5">
+        <v>30101</v>
+      </c>
+      <c r="H19" s="20">
+        <v>0.17341616557589448</v>
+      </c>
+      <c r="I19" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J19" s="5">
+        <v>28155</v>
+      </c>
+      <c r="K19" s="20">
+        <v>0.25451962351269758</v>
+      </c>
+      <c r="L19" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M19" s="5">
+        <v>28155</v>
+      </c>
+      <c r="N19" s="20">
+        <v>0.25451962351269758</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5">
+        <v>534</v>
+      </c>
+      <c r="D20" s="5">
+        <v>100</v>
+      </c>
+      <c r="E20" s="5">
+        <v>41340</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J20" s="5">
+        <v>28406</v>
+      </c>
+      <c r="K20" s="20">
+        <v>0.4553263395057382</v>
+      </c>
+      <c r="L20" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M20" s="5">
+        <v>28406</v>
+      </c>
+      <c r="N20" s="20">
+        <v>0.4553263395057382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5">
+        <v>526</v>
+      </c>
+      <c r="D21" s="5">
+        <v>100</v>
+      </c>
+      <c r="E21" s="5">
+        <v>62818</v>
+      </c>
+      <c r="F21" s="5">
+        <v>41035</v>
+      </c>
+      <c r="G21" s="5">
+        <v>46704</v>
+      </c>
+      <c r="H21" s="20">
+        <v>0.34502398081534774</v>
+      </c>
+      <c r="I21" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J21" s="5">
+        <v>38137</v>
+      </c>
+      <c r="K21" s="20">
+        <v>0.64716679340273231</v>
+      </c>
+      <c r="L21" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M21" s="5">
+        <v>38511</v>
+      </c>
+      <c r="N21" s="20">
+        <v>0.63117031497494225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5">
+        <v>203</v>
+      </c>
+      <c r="D22" s="5">
+        <v>43</v>
+      </c>
+      <c r="E22" s="5">
+        <v>22545</v>
+      </c>
+      <c r="F22" s="5">
+        <v>43150</v>
+      </c>
+      <c r="G22" s="5">
+        <v>22327</v>
+      </c>
+      <c r="H22" s="20">
+        <v>9.763962914856452E-3</v>
+      </c>
+      <c r="I22" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J22" s="5">
+        <v>738</v>
+      </c>
+      <c r="K22" s="20">
+        <v>29.548780487804876</v>
+      </c>
+      <c r="L22" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M22" s="5">
+        <v>788</v>
+      </c>
+      <c r="N22" s="20">
+        <v>27.610406091370557</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="5">
+        <v>198</v>
+      </c>
+      <c r="D23" s="5">
+        <v>43</v>
+      </c>
+      <c r="E23" s="5">
+        <v>22841</v>
+      </c>
+      <c r="F23" s="5">
+        <v>43132</v>
+      </c>
+      <c r="G23" s="5">
+        <v>22381</v>
+      </c>
+      <c r="H23" s="20">
+        <v>2.0463786247263305E-2</v>
+      </c>
+      <c r="I23" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J23" s="5">
+        <v>749</v>
+      </c>
+      <c r="K23" s="20">
+        <v>29.495327102803738</v>
+      </c>
+      <c r="L23" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M23" s="5">
+        <v>877</v>
+      </c>
+      <c r="N23" s="20">
+        <v>25.044469783352337</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="5">
+        <v>211</v>
+      </c>
+      <c r="D24" s="5">
+        <v>43</v>
+      </c>
+      <c r="E24" s="5">
+        <v>23122</v>
+      </c>
+      <c r="F24" s="5">
+        <v>43058</v>
+      </c>
+      <c r="G24" s="5">
+        <v>22540</v>
+      </c>
+      <c r="H24" s="20">
+        <v>2.5687666370896183E-2</v>
+      </c>
+      <c r="I24" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J24" s="5">
+        <v>898</v>
+      </c>
+      <c r="K24" s="20">
+        <v>24.748329621380847</v>
+      </c>
+      <c r="L24" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M24" s="5">
+        <v>906</v>
+      </c>
+      <c r="N24" s="20">
+        <v>24.520971302428258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="5">
+        <v>204</v>
+      </c>
+      <c r="D25" s="5">
+        <v>43</v>
+      </c>
+      <c r="E25" s="5">
+        <v>66857</v>
+      </c>
+      <c r="F25" s="5">
+        <v>43193</v>
+      </c>
+      <c r="G25" s="5">
+        <v>45396</v>
+      </c>
+      <c r="H25" s="20">
+        <v>0.47255264781037976</v>
+      </c>
+      <c r="I25" s="5">
+        <v>4470</v>
+      </c>
+      <c r="J25" s="5">
+        <v>66846</v>
+      </c>
+      <c r="K25" s="20">
+        <v>2.9919516500613349E-5</v>
+      </c>
+      <c r="L25" s="5">
+        <v>333.02</v>
+      </c>
+      <c r="M25" s="5">
+        <v>66846</v>
+      </c>
+      <c r="N25" s="20">
+        <v>2.9919516500613349E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5">
+        <v>510</v>
+      </c>
+      <c r="D26" s="5">
+        <v>99</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1474</v>
+      </c>
+      <c r="F26" s="5">
+        <v>38567</v>
+      </c>
+      <c r="G26" s="5">
+        <v>800</v>
+      </c>
+      <c r="H26" s="20">
+        <v>0.80249999999999999</v>
+      </c>
+      <c r="I26" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J26" s="5">
+        <v>632</v>
+      </c>
+      <c r="K26" s="20">
+        <v>1.3322784810126582</v>
+      </c>
+      <c r="L26" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M26" s="5">
+        <v>632</v>
+      </c>
+      <c r="N26" s="20">
+        <v>1.3322784810126582</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="5">
+        <v>208</v>
+      </c>
+      <c r="D27" s="5">
+        <v>41</v>
+      </c>
+      <c r="E27" s="5">
+        <v>232</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1292.07</v>
+      </c>
+      <c r="G27" s="5">
+        <v>202</v>
+      </c>
+      <c r="H27" s="20">
+        <v>0.14851485148514851</v>
+      </c>
+      <c r="I27" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J27" s="5">
+        <v>149</v>
+      </c>
+      <c r="K27" s="20">
+        <v>0.55704697986577179</v>
+      </c>
+      <c r="L27" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M27" s="5">
+        <v>153</v>
+      </c>
+      <c r="N27" s="20">
+        <v>0.5163398692810458</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5">
+        <v>255</v>
+      </c>
+      <c r="D28" s="5">
+        <v>49</v>
+      </c>
+      <c r="E28" s="5">
+        <v>282</v>
+      </c>
+      <c r="F28" s="5">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="G28" s="5">
+        <v>282</v>
+      </c>
+      <c r="H28" s="20">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="J28" s="5">
+        <v>272</v>
+      </c>
+      <c r="K28" s="20">
+        <v>3.6764705882352942E-2</v>
+      </c>
+      <c r="L28" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="M28" s="5">
+        <v>272</v>
+      </c>
+      <c r="N28" s="20">
+        <v>3.6764705882352942E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="5">
+        <v>259</v>
+      </c>
+      <c r="D29" s="5">
+        <v>51</v>
+      </c>
+      <c r="E29" s="5">
+        <v>378</v>
+      </c>
+      <c r="F29" s="5">
+        <v>26.46</v>
+      </c>
+      <c r="G29" s="5">
+        <v>378</v>
+      </c>
+      <c r="H29" s="20">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="J29" s="5">
+        <v>372</v>
+      </c>
+      <c r="K29" s="20">
+        <v>1.6129032258064516E-2</v>
+      </c>
+      <c r="L29" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="M29" s="5">
+        <v>372</v>
+      </c>
+      <c r="N29" s="20">
+        <v>1.6129032258064516E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="5">
+        <v>573</v>
+      </c>
+      <c r="D30" s="5">
+        <v>110</v>
+      </c>
+      <c r="E30" s="5">
+        <v>848</v>
+      </c>
+      <c r="F30" s="5">
+        <v>83.23</v>
+      </c>
+      <c r="G30" s="5">
+        <v>848</v>
+      </c>
+      <c r="H30" s="20">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>2407</v>
+      </c>
+      <c r="J30" s="5">
+        <v>812</v>
+      </c>
+      <c r="K30" s="20">
+        <v>4.4334975369458129E-2</v>
+      </c>
+      <c r="L30" s="5">
+        <v>682</v>
+      </c>
+      <c r="M30" s="5">
+        <v>809</v>
+      </c>
+      <c r="N30" s="20">
+        <v>4.8207663782447466E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="5">
+        <v>871</v>
+      </c>
+      <c r="D31" s="5">
+        <v>151</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1415</v>
+      </c>
+      <c r="F31" s="5">
+        <v>29094.62</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1414</v>
+      </c>
+      <c r="H31" s="20">
+        <v>7.0721357850070724E-4</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="J31" s="5">
+        <v>1353</v>
+      </c>
+      <c r="K31" s="20">
+        <v>4.5824094604582408E-2</v>
+      </c>
+      <c r="L31" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="M31" s="5">
+        <v>1353</v>
+      </c>
+      <c r="N31" s="20">
+        <v>4.5824094604582408E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>30</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="5">
+        <v>962</v>
+      </c>
+      <c r="D32" s="5">
+        <v>175</v>
+      </c>
+      <c r="E32" s="5">
+        <v>1644</v>
+      </c>
+      <c r="F32" s="5">
+        <v>5413.79</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1641</v>
+      </c>
+      <c r="H32" s="20">
+        <v>1.8281535648994515E-3</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="J32" s="5">
+        <v>1568</v>
+      </c>
+      <c r="K32" s="20">
+        <v>4.8469387755102039E-2</v>
+      </c>
+      <c r="L32" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="M32" s="5">
+        <v>1568</v>
+      </c>
+      <c r="N32" s="20">
+        <v>4.8469387755102039E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>31</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1389</v>
+      </c>
+      <c r="D33" s="5">
+        <v>254</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2376</v>
+      </c>
+      <c r="F33" s="5">
+        <v>43159</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2369</v>
+      </c>
+      <c r="H33" s="20">
+        <v>1.2663571127057829E-3</v>
+      </c>
+      <c r="I33" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="J33" s="5">
+        <v>2269</v>
+      </c>
+      <c r="K33" s="20">
+        <v>4.7157338034376377E-2</v>
+      </c>
+      <c r="L33" s="5">
+        <v>1.42</v>
+      </c>
+      <c r="M33" s="5">
+        <v>2269</v>
+      </c>
+      <c r="N33" s="20">
+        <v>4.7157338034376377E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>32</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1825</v>
+      </c>
+      <c r="D34" s="5">
+        <v>324</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2547</v>
+      </c>
+      <c r="F34" s="5">
+        <v>40499.300000000003</v>
+      </c>
+      <c r="G34" s="5">
+        <v>2533</v>
+      </c>
+      <c r="H34" s="20">
+        <v>5.5270430319778914E-3</v>
+      </c>
+      <c r="I34" s="5">
+        <v>2</v>
+      </c>
+      <c r="J34" s="5">
+        <v>2448</v>
+      </c>
+      <c r="K34" s="20">
+        <v>4.0441176470588237E-2</v>
+      </c>
+      <c r="L34" s="5">
+        <v>3.59</v>
+      </c>
+      <c r="M34" s="5">
+        <v>2448</v>
+      </c>
+      <c r="N34" s="20">
+        <v>4.0441176470588237E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>33</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1822</v>
+      </c>
+      <c r="D35" s="5">
+        <v>342</v>
+      </c>
+      <c r="E35" s="5">
+        <v>2101</v>
+      </c>
+      <c r="F35" s="5">
+        <v>30687</v>
+      </c>
+      <c r="G35" s="5">
+        <v>2064</v>
+      </c>
+      <c r="H35" s="20">
+        <v>1.4050387596899225E-2</v>
+      </c>
+      <c r="I35" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J35" s="5">
+        <v>1840</v>
+      </c>
+      <c r="K35" s="20">
+        <v>0.14184782608695654</v>
+      </c>
+      <c r="L35" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M35" s="5">
+        <v>1840</v>
+      </c>
+      <c r="N35" s="20">
+        <v>0.14184782608695654</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1967</v>
+      </c>
+      <c r="D36" s="5">
+        <v>359</v>
+      </c>
+      <c r="E36" s="5">
+        <v>2080</v>
+      </c>
+      <c r="F36" s="5">
+        <v>32215</v>
+      </c>
+      <c r="G36" s="5">
+        <v>2021</v>
+      </c>
+      <c r="H36" s="20">
+        <v>2.3750618505690251E-2</v>
+      </c>
+      <c r="I36" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J36" s="5">
+        <v>1933</v>
+      </c>
+      <c r="K36" s="20">
+        <v>7.6047594412829794E-2</v>
+      </c>
+      <c r="L36" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M36" s="5">
+        <v>1933</v>
+      </c>
+      <c r="N36" s="20">
+        <v>7.6047594412829794E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>35</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1973</v>
+      </c>
+      <c r="D37" s="5">
+        <v>379</v>
+      </c>
+      <c r="E37" s="5">
+        <v>2307</v>
+      </c>
+      <c r="F37" s="5">
+        <v>42279</v>
+      </c>
+      <c r="G37" s="5">
+        <v>2231</v>
+      </c>
+      <c r="H37" s="20">
+        <v>2.3756163155535633E-2</v>
+      </c>
+      <c r="I37" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J37" s="5">
+        <v>2032</v>
+      </c>
+      <c r="K37" s="20">
+        <v>0.13533464566929135</v>
+      </c>
+      <c r="L37" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M37" s="5">
+        <v>2031</v>
+      </c>
+      <c r="N37" s="20">
+        <v>0.13589364844903989</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="5">
+        <v>256</v>
+      </c>
+      <c r="D38" s="5">
+        <v>48</v>
+      </c>
+      <c r="E38" s="5">
+        <v>13135</v>
+      </c>
+      <c r="F38" s="5">
+        <v>43141</v>
+      </c>
+      <c r="G38" s="5">
+        <v>12125</v>
+      </c>
+      <c r="H38" s="20">
+        <v>8.3298969072164955E-2</v>
+      </c>
+      <c r="I38" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J38" s="5">
+        <v>10739</v>
+      </c>
+      <c r="K38" s="20">
+        <v>0.22311202160350127</v>
+      </c>
+      <c r="L38" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M38" s="5">
+        <v>10764</v>
+      </c>
+      <c r="N38" s="20">
+        <v>0.2202712746191007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>37</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="5">
+        <v>250</v>
+      </c>
+      <c r="D39" s="5">
+        <v>48</v>
+      </c>
+      <c r="E39" s="5">
+        <v>13802</v>
+      </c>
+      <c r="F39" s="5">
+        <v>43033</v>
+      </c>
+      <c r="G39" s="5">
+        <v>12130</v>
+      </c>
+      <c r="H39" s="20">
+        <v>0.13784006595218468</v>
+      </c>
+      <c r="I39" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J39" s="5">
+        <v>10912</v>
+      </c>
+      <c r="K39" s="20">
+        <v>0.26484604105571846</v>
+      </c>
+      <c r="L39" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M39" s="5">
+        <v>11000</v>
+      </c>
+      <c r="N39" s="20">
+        <v>0.25472727272727275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="5">
+        <v>254</v>
+      </c>
+      <c r="D40" s="5">
+        <v>48</v>
+      </c>
+      <c r="E40" s="5">
+        <v>16540</v>
+      </c>
+      <c r="F40" s="5">
+        <v>43102</v>
+      </c>
+      <c r="G40" s="5">
+        <v>13096</v>
+      </c>
+      <c r="H40" s="20">
+        <v>0.26298106291997558</v>
+      </c>
+      <c r="I40" s="5">
+        <v>36000</v>
+      </c>
+      <c r="J40" s="5">
+        <v>11732</v>
+      </c>
+      <c r="K40" s="20">
+        <v>0.40981929764745995</v>
+      </c>
+      <c r="L40" s="5">
+        <v>36000</v>
+      </c>
+      <c r="M40" s="5">
+        <v>11822</v>
+      </c>
+      <c r="N40" s="20">
+        <v>0.39908644899340212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="5">
+        <v>249</v>
+      </c>
+      <c r="D41" s="5">
+        <v>48</v>
+      </c>
+      <c r="E41" s="5">
+        <v>25977</v>
+      </c>
+      <c r="F41" s="5">
+        <v>43057</v>
+      </c>
+      <c r="G41" s="5">
+        <v>22266</v>
+      </c>
+      <c r="H41" s="20">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I41" s="5">
+        <v>18677</v>
+      </c>
+      <c r="J41" s="5">
+        <v>25037</v>
+      </c>
+      <c r="K41" s="20">
+        <v>3.7544434237328755E-2</v>
+      </c>
+      <c r="L41" s="5">
+        <v>1401</v>
+      </c>
+      <c r="M41" s="5">
+        <v>25043</v>
+      </c>
+      <c r="N41" s="20">
+        <v>3.7295851136045999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F20:H20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>